<commit_message>
Updated sprint backlog for tuesday
Updated sprint backlog to show work done so far
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint2_Backlog-1.xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint2_Backlog-1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22601"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_2418\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_186\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4A5D46E-C517-447E-B8A6-C04FD02C005A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F359C66F-8C0F-4DDF-A3B4-5EC0580D5EF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="80">
   <si>
     <t>AGILE SPRINT BACKLOG TEMPLATE WITH BURNDOWN CHART</t>
   </si>
@@ -116,9 +116,6 @@
     <t>Generation of SQL Method(s)</t>
   </si>
   <si>
-    <t>Pending Review</t>
-  </si>
-  <si>
     <t>Generation of JavaCode</t>
   </si>
   <si>
@@ -129,6 +126,9 @@
   </si>
   <si>
     <t>Implementation on frontend</t>
+  </si>
+  <si>
+    <t>A.R.</t>
   </si>
   <si>
     <t>The database should contain queries for the different procedure searches.</t>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>Generarton of Java Related Code</t>
+  </si>
+  <si>
+    <t>R.C/H.Z</t>
   </si>
   <si>
     <t>Generation Of testing</t>
@@ -191,10 +194,85 @@
     <t>Implementing animations in website</t>
   </si>
   <si>
-    <t>CH</t>
+    <t>Table cell click behaves like marker click</t>
   </si>
   <si>
-    <t>User Story #6</t>
+    <t>Create test functions for search SQL procedures via distance.</t>
+  </si>
+  <si>
+    <t>SQL procedure does not return an empty table</t>
+  </si>
+  <si>
+    <t>SQL procedure does not return rows of different sizes</t>
+  </si>
+  <si>
+    <t>SQL procedure does not return any null entries or empty strings</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>As a client, I want to see a color associated with the procedure's cost</t>
+  </si>
+  <si>
+    <t>Implimenting javascript to change cost colour with hard-coded values</t>
+  </si>
+  <si>
+    <t>F.S</t>
+  </si>
+  <si>
+    <t>Recieving cost of procedure from SQL</t>
+  </si>
+  <si>
+    <t>As a client, I want to see the facilities rating when I click it's marker</t>
+  </si>
+  <si>
+    <t>Implimenting hard-coded javascript to display star rating</t>
+  </si>
+  <si>
+    <t>Refacotring code to use actual values</t>
+  </si>
+  <si>
+    <t>Create test functions for search SQL procedures via cost.</t>
+  </si>
+  <si>
+    <t>SQL procedure does not return any null entries or empty entries</t>
+  </si>
+  <si>
+    <t>Procedure returns costs between the limits</t>
+  </si>
+  <si>
+    <t>Procedure returns reviews above the minimum</t>
+  </si>
+  <si>
+    <t>Refacotring geocoding to use data from SQL</t>
+  </si>
+  <si>
+    <t>Recieve lat/long from database</t>
+  </si>
+  <si>
+    <t>Replace geocoding address with lat/long</t>
+  </si>
+  <si>
+    <t>Calculating distance between client location and hospital locations</t>
+  </si>
+  <si>
+    <t>Returning a hospital list with distances associated with each hospital relative to users's location.</t>
+  </si>
+  <si>
+    <t>Day 1 Notes:</t>
+  </si>
+  <si>
+    <t>C.H - I had trouble with the eclipse workspace until late in the day so couldnt test any changes made to the website. worked on documentation in paralell</t>
+  </si>
+  <si>
+    <t>Day 2 Notes:</t>
+  </si>
+  <si>
+    <t>C.H - New user stories were considered so I updated the sprint backlog accordingly</t>
+  </si>
+  <si>
+    <t>R.C - Updated Methods to reflect more accurate information, Meaning re-evaluation of esitmated time</t>
   </si>
   <si>
     <t xml:space="preserve">Any articles, templates, or information provided by Smartsheet on the website are for reference only. While we strive to keep the information up to date and correct, we make no representations or warranties of any kind, express or implied, about the completeness, accuracy, reliability, suitability, or availability with respect to the website or the information, articles, templates, or related graphics contained on the website. Any reliance you place on such information is therefore strictly at your own risk. </t>
@@ -711,15 +789,15 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Agile Sprint 2 Backlog '!$F$41:$G$41</c:f>
+              <c:f>'Agile Sprint 2 Backlog '!$F$62:$G$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>37.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1288,7 +1366,7 @@
   <dimension ref="B1:AB124"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="D2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="B7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -5305,11 +5383,11 @@
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AB133"/>
+  <dimension ref="B1:AB156"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O36" sqref="O36"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.15"/>
@@ -5462,7 +5540,9 @@
       <c r="G4" s="9">
         <v>1</v>
       </c>
-      <c r="H4" s="9"/>
+      <c r="H4" s="9">
+        <v>1</v>
+      </c>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
@@ -5495,7 +5575,7 @@
         <v>23</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F5" s="9">
         <v>2</v>
@@ -5503,7 +5583,9 @@
       <c r="G5" s="9">
         <v>1</v>
       </c>
-      <c r="H5" s="9"/>
+      <c r="H5" s="9">
+        <v>0</v>
+      </c>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
@@ -5527,16 +5609,26 @@
     </row>
     <row r="6" spans="2:28" ht="25.15" customHeight="1">
       <c r="B6" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="9">
         <v>1</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="D6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="9">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0</v>
+      </c>
+      <c r="H6" s="9">
+        <v>1</v>
+      </c>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
@@ -5560,18 +5652,26 @@
     </row>
     <row r="7" spans="2:28" ht="25.15" customHeight="1">
       <c r="B7" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="9">
         <v>1</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+        <v>28</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="9">
+        <v>2</v>
+      </c>
+      <c r="G7" s="9">
+        <v>1</v>
+      </c>
+      <c r="H7" s="9">
+        <v>1</v>
+      </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
@@ -5595,16 +5695,26 @@
     </row>
     <row r="8" spans="2:28" ht="25.15" customHeight="1">
       <c r="B8" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="9">
         <v>1</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
+      <c r="D8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="9">
+        <v>1</v>
+      </c>
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
+      <c r="H8" s="9">
+        <v>1</v>
+      </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
@@ -5676,7 +5786,9 @@
       <c r="G10" s="9">
         <v>3</v>
       </c>
-      <c r="H10" s="9"/>
+      <c r="H10" s="9">
+        <v>4</v>
+      </c>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
@@ -5700,7 +5812,7 @@
     </row>
     <row r="11" spans="2:28" ht="25.15" customHeight="1">
       <c r="B11" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="9">
         <v>2</v>
@@ -5733,7 +5845,7 @@
     </row>
     <row r="12" spans="2:28" ht="25.15" customHeight="1">
       <c r="B12" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="9">
         <v>2</v>
@@ -5772,7 +5884,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
@@ -5841,7 +5953,7 @@
         <v>36</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F15" s="9">
         <v>1</v>
@@ -5878,10 +5990,18 @@
       <c r="C16" s="9">
         <v>2</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
+      <c r="D16" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="9">
+        <v>1</v>
+      </c>
+      <c r="G16" s="9">
+        <v>1</v>
+      </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
@@ -5906,16 +6026,24 @@
     </row>
     <row r="17" spans="2:28" ht="25.15" customHeight="1">
       <c r="B17" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="9">
         <v>2</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="D17" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="9">
+        <v>1</v>
+      </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
+      <c r="H17" s="9">
+        <v>1</v>
+      </c>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
@@ -5939,15 +6067,17 @@
     </row>
     <row r="18" spans="2:28" ht="25.15" customHeight="1">
       <c r="B18" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C18" s="9">
         <v>2</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="9"/>
+        <v>28</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
@@ -5974,7 +6104,7 @@
     </row>
     <row r="19" spans="2:28" ht="38.25">
       <c r="B19" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
@@ -6007,13 +6137,13 @@
     </row>
     <row r="20" spans="2:28" ht="25.15" customHeight="1">
       <c r="B20" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C20" s="9">
         <v>1</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>33</v>
@@ -6048,7 +6178,7 @@
     </row>
     <row r="21" spans="2:28" ht="25.15" customHeight="1">
       <c r="B21" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -6079,7 +6209,7 @@
     </row>
     <row r="22" spans="2:28" ht="25.15" customHeight="1">
       <c r="B22" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -6141,7 +6271,7 @@
     </row>
     <row r="24" spans="2:28" ht="25.15" customHeight="1">
       <c r="B24" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
@@ -6172,13 +6302,13 @@
     </row>
     <row r="25" spans="2:28" ht="25.15" customHeight="1">
       <c r="B25" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C25" s="9">
         <v>1</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>24</v>
@@ -6189,7 +6319,9 @@
       <c r="G25" s="9">
         <v>1</v>
       </c>
-      <c r="H25" s="9"/>
+      <c r="H25" s="9">
+        <v>0</v>
+      </c>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -6213,7 +6345,7 @@
     </row>
     <row r="26" spans="2:28" ht="25.15" customHeight="1">
       <c r="B26" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
@@ -6306,7 +6438,7 @@
     </row>
     <row r="29" spans="2:28" ht="34.9" customHeight="1">
       <c r="B29" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="8"/>
@@ -6335,15 +6467,15 @@
       <c r="AA29" s="4"/>
       <c r="AB29" s="4"/>
     </row>
-    <row r="30" spans="2:28" ht="13.5">
+    <row r="30" spans="2:28" ht="18" customHeight="1">
       <c r="B30" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C30" s="9">
         <v>1</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E30" s="9" t="s">
         <v>33</v>
@@ -6354,7 +6486,9 @@
       <c r="G30" s="9">
         <v>2</v>
       </c>
-      <c r="H30" s="9"/>
+      <c r="H30" s="9">
+        <v>1</v>
+      </c>
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
@@ -6378,13 +6512,13 @@
     </row>
     <row r="31" spans="2:28" ht="14.25" customHeight="1">
       <c r="B31" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C31" s="9">
         <v>2</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>33</v>
@@ -6395,7 +6529,9 @@
       <c r="G31" s="9">
         <v>5</v>
       </c>
-      <c r="H31" s="9"/>
+      <c r="H31" s="9">
+        <v>4</v>
+      </c>
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
@@ -6419,14 +6555,26 @@
     </row>
     <row r="32" spans="2:28" ht="13.5">
       <c r="B32" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
+        <v>52</v>
+      </c>
+      <c r="C32" s="9">
+        <v>2</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" s="9">
+        <v>2</v>
+      </c>
+      <c r="G32" s="9">
+        <v>0</v>
+      </c>
+      <c r="H32" s="9">
+        <v>3</v>
+      </c>
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -6448,7 +6596,7 @@
       <c r="AA32" s="4"/>
       <c r="AB32" s="4"/>
     </row>
-    <row r="33" spans="2:28" ht="13.5">
+    <row r="33" spans="2:28" ht="12.75">
       <c r="B33" s="9" t="s">
         <v>14</v>
       </c>
@@ -6479,7 +6627,7 @@
       <c r="AA33" s="4"/>
       <c r="AB33" s="4"/>
     </row>
-    <row r="34" spans="2:28" ht="13.5">
+    <row r="34" spans="2:28" ht="12.75">
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
@@ -6510,7 +6658,7 @@
     </row>
     <row r="35" spans="2:28" ht="34.9" customHeight="1">
       <c r="B35" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="8"/>
@@ -6539,16 +6687,28 @@
       <c r="AA35" s="4"/>
       <c r="AB35" s="4"/>
     </row>
-    <row r="36" spans="2:28" ht="13.5">
+    <row r="36" spans="2:28" ht="12.75">
       <c r="B36" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
+        <v>54</v>
+      </c>
+      <c r="C36" s="9">
+        <v>1</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F36" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G36" s="9">
+        <v>0</v>
+      </c>
+      <c r="H36" s="9">
+        <v>0.5</v>
+      </c>
       <c r="I36" s="9"/>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
@@ -6572,14 +6732,26 @@
     </row>
     <row r="37" spans="2:28" ht="14.25" customHeight="1">
       <c r="B37" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
+        <v>55</v>
+      </c>
+      <c r="C37" s="9">
+        <v>1</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G37" s="9">
+        <v>0</v>
+      </c>
+      <c r="H37" s="9">
+        <v>0.5</v>
+      </c>
       <c r="I37" s="9"/>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
@@ -6601,16 +6773,28 @@
       <c r="AA37" s="4"/>
       <c r="AB37" s="4"/>
     </row>
-    <row r="38" spans="2:28" ht="13.5">
+    <row r="38" spans="2:28" ht="25.5">
       <c r="B38" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
+        <v>56</v>
+      </c>
+      <c r="C38" s="9">
+        <v>1</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G38" s="9">
+        <v>0</v>
+      </c>
+      <c r="H38" s="9">
+        <v>0.5</v>
+      </c>
       <c r="I38" s="9"/>
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
@@ -6633,15 +6817,23 @@
       <c r="AB38" s="4"/>
     </row>
     <row r="39" spans="2:28" ht="13.5">
-      <c r="B39" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9">
+        <v>1</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F39" s="9">
+        <v>0.5</v>
+      </c>
       <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
+      <c r="H39" s="9">
+        <v>1</v>
+      </c>
       <c r="I39" s="9"/>
       <c r="J39" s="9"/>
       <c r="K39" s="9"/>
@@ -6665,12 +6857,22 @@
     </row>
     <row r="40" spans="2:28" ht="13.5">
       <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
+      <c r="C40" s="9">
+        <v>1</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F40" s="9">
+        <v>0.5</v>
+      </c>
       <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
+      <c r="H40" s="9">
+        <v>0.5</v>
+      </c>
       <c r="I40" s="9"/>
       <c r="J40" s="9"/>
       <c r="K40" s="9"/>
@@ -6692,41 +6894,20 @@
       <c r="AA40" s="4"/>
       <c r="AB40" s="4"/>
     </row>
-    <row r="41" spans="2:28" ht="12.75">
-      <c r="B41" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5">
-        <f>SUM(F4:F40)</f>
-        <v>19</v>
-      </c>
-      <c r="G41" s="5">
-        <f>SUM(G4:G40)</f>
-        <v>19</v>
-      </c>
-      <c r="H41" s="5">
-        <f>SUM(H4:H40)</f>
-        <v>0</v>
-      </c>
-      <c r="I41" s="5">
-        <f>SUM(I4:I40)</f>
-        <v>0</v>
-      </c>
-      <c r="J41" s="5">
-        <f>SUM(J3:J40)</f>
-        <v>0</v>
-      </c>
-      <c r="K41" s="5">
-        <f>SUM(K9:K40)</f>
-        <v>0</v>
-      </c>
-      <c r="L41" s="5">
-        <f>SUM(L9:L40)</f>
-        <v>0</v>
-      </c>
+    <row r="41" spans="2:28" ht="26.25" customHeight="1">
+      <c r="B41" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="7"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
@@ -6744,18 +6925,30 @@
       <c r="AA41" s="4"/>
       <c r="AB41" s="4"/>
     </row>
-    <row r="42" spans="2:28" ht="12.75">
-      <c r="B42" s="4"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="4"/>
+    <row r="42" spans="2:28" ht="25.5">
+      <c r="B42" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="9">
+        <v>1</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F42" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G42" s="9">
+        <v>1</v>
+      </c>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
@@ -6774,17 +6967,29 @@
       <c r="AB42" s="4"/>
     </row>
     <row r="43" spans="2:28" ht="12.75">
-      <c r="B43" s="4"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
-      <c r="L43" s="4"/>
+      <c r="B43" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="9">
+        <v>1</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F43" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G43" s="9">
+        <v>0</v>
+      </c>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
       <c r="M43" s="4"/>
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
@@ -6803,17 +7008,19 @@
       <c r="AB43" s="4"/>
     </row>
     <row r="44" spans="2:28" ht="12.75">
-      <c r="B44" s="4"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
+      <c r="B44" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="9"/>
       <c r="M44" s="4"/>
       <c r="N44" s="4"/>
       <c r="O44" s="4"/>
@@ -6832,17 +7039,19 @@
       <c r="AB44" s="4"/>
     </row>
     <row r="45" spans="2:28" ht="12.75">
-      <c r="B45" s="4"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
-      <c r="L45" s="4"/>
+      <c r="B45" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="9"/>
       <c r="M45" s="4"/>
       <c r="N45" s="4"/>
       <c r="O45" s="4"/>
@@ -6860,18 +7069,20 @@
       <c r="AA45" s="4"/>
       <c r="AB45" s="4"/>
     </row>
-    <row r="46" spans="2:28" ht="12.75">
-      <c r="B46" s="4"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="4"/>
+    <row r="46" spans="2:28" ht="25.5">
+      <c r="B46" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="7"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
       <c r="M46" s="4"/>
       <c r="N46" s="4"/>
       <c r="O46" s="4"/>
@@ -6889,18 +7100,30 @@
       <c r="AA46" s="4"/>
       <c r="AB46" s="4"/>
     </row>
-    <row r="47" spans="2:28" ht="12.75">
-      <c r="B47" s="4"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
+    <row r="47" spans="2:28" ht="25.5">
+      <c r="B47" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" s="9">
+        <v>1</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F47" s="9">
+        <v>1</v>
+      </c>
+      <c r="G47" s="9">
+        <v>1</v>
+      </c>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
       <c r="M47" s="4"/>
       <c r="N47" s="4"/>
       <c r="O47" s="4"/>
@@ -6919,17 +7142,29 @@
       <c r="AB47" s="4"/>
     </row>
     <row r="48" spans="2:28" ht="12.75">
-      <c r="B48" s="4"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
+      <c r="B48" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" s="9">
+        <v>1</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F48" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G48" s="9">
+        <v>0</v>
+      </c>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
       <c r="O48" s="4"/>
@@ -6948,17 +7183,19 @@
       <c r="AB48" s="4"/>
     </row>
     <row r="49" spans="2:28" ht="12.75">
-      <c r="B49" s="4"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
+      <c r="B49" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="9"/>
+      <c r="K49" s="9"/>
+      <c r="L49" s="9"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
       <c r="O49" s="4"/>
@@ -6977,17 +7214,19 @@
       <c r="AB49" s="4"/>
     </row>
     <row r="50" spans="2:28" ht="12.75">
-      <c r="B50" s="4"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
-      <c r="L50" s="4"/>
+      <c r="B50" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
       <c r="O50" s="4"/>
@@ -7005,18 +7244,20 @@
       <c r="AA50" s="4"/>
       <c r="AB50" s="4"/>
     </row>
-    <row r="51" spans="2:28" ht="12.75">
-      <c r="B51" s="4"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
-      <c r="H51" s="4"/>
-      <c r="I51" s="4"/>
-      <c r="J51" s="4"/>
-      <c r="K51" s="4"/>
-      <c r="L51" s="4"/>
+    <row r="51" spans="2:28" ht="25.5">
+      <c r="B51" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" s="7"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="8"/>
+      <c r="J51" s="8"/>
+      <c r="K51" s="8"/>
+      <c r="L51" s="8"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
       <c r="O51" s="4"/>
@@ -7035,17 +7276,31 @@
       <c r="AB51" s="4"/>
     </row>
     <row r="52" spans="2:28" ht="12.75">
-      <c r="B52" s="4"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
-      <c r="H52" s="4"/>
-      <c r="I52" s="4"/>
-      <c r="J52" s="4"/>
-      <c r="K52" s="4"/>
-      <c r="L52" s="4"/>
+      <c r="B52" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" s="9">
+        <v>1</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F52" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G52" s="9">
+        <v>0</v>
+      </c>
+      <c r="H52" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I52" s="9"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="9"/>
+      <c r="L52" s="9"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
       <c r="O52" s="4"/>
@@ -7063,18 +7318,32 @@
       <c r="AA52" s="4"/>
       <c r="AB52" s="4"/>
     </row>
-    <row r="53" spans="2:28" ht="12.75">
-      <c r="B53" s="4"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4"/>
-      <c r="J53" s="4"/>
-      <c r="K53" s="4"/>
-      <c r="L53" s="4"/>
+    <row r="53" spans="2:28" ht="25.5">
+      <c r="B53" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" s="9">
+        <v>1</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F53" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G53" s="9">
+        <v>0</v>
+      </c>
+      <c r="H53" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I53" s="9"/>
+      <c r="J53" s="9"/>
+      <c r="K53" s="9"/>
+      <c r="L53" s="9"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
       <c r="O53" s="4"/>
@@ -7092,18 +7361,32 @@
       <c r="AA53" s="4"/>
       <c r="AB53" s="4"/>
     </row>
-    <row r="54" spans="2:28" ht="12.75">
-      <c r="B54" s="4"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
+    <row r="54" spans="2:28" ht="25.5">
+      <c r="B54" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C54" s="9">
+        <v>1</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F54" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G54" s="9">
+        <v>0</v>
+      </c>
+      <c r="H54" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="9"/>
+      <c r="L54" s="9"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
       <c r="O54" s="4"/>
@@ -7121,18 +7404,30 @@
       <c r="AA54" s="4"/>
       <c r="AB54" s="4"/>
     </row>
-    <row r="55" spans="2:28" ht="12.75">
-      <c r="B55" s="4"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
-      <c r="L55" s="4"/>
+    <row r="55" spans="2:28" ht="27">
+      <c r="B55" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C55" s="9">
+        <v>1</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F55" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9">
+        <v>1</v>
+      </c>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9"/>
+      <c r="K55" s="9"/>
+      <c r="L55" s="9"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
       <c r="O55" s="4"/>
@@ -7150,18 +7445,30 @@
       <c r="AA55" s="4"/>
       <c r="AB55" s="4"/>
     </row>
-    <row r="56" spans="2:28" ht="12.75">
-      <c r="B56" s="4"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="4"/>
-      <c r="I56" s="4"/>
-      <c r="J56" s="4"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="4"/>
+    <row r="56" spans="2:28" ht="27">
+      <c r="B56" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56" s="9">
+        <v>1</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F56" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="9"/>
+      <c r="L56" s="9"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
       <c r="O56" s="4"/>
@@ -7179,18 +7486,20 @@
       <c r="AA56" s="4"/>
       <c r="AB56" s="4"/>
     </row>
-    <row r="57" spans="2:28" ht="12.75">
-      <c r="B57" s="4"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
-      <c r="K57" s="4"/>
-      <c r="L57" s="4"/>
+    <row r="57" spans="2:28" ht="25.5">
+      <c r="B57" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C57" s="7"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="8"/>
+      <c r="K57" s="8"/>
+      <c r="L57" s="8"/>
       <c r="M57" s="4"/>
       <c r="N57" s="4"/>
       <c r="O57" s="4"/>
@@ -7208,18 +7517,32 @@
       <c r="AA57" s="4"/>
       <c r="AB57" s="4"/>
     </row>
-    <row r="58" spans="2:28" ht="12.75">
-      <c r="B58" s="4"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
-      <c r="H58" s="4"/>
-      <c r="I58" s="4"/>
-      <c r="J58" s="4"/>
-      <c r="K58" s="4"/>
-      <c r="L58" s="4"/>
+    <row r="58" spans="2:28" ht="13.5">
+      <c r="B58" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C58" s="9">
+        <v>1</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F58" s="9">
+        <v>1</v>
+      </c>
+      <c r="G58" s="9">
+        <v>0</v>
+      </c>
+      <c r="H58" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9"/>
+      <c r="K58" s="9"/>
+      <c r="L58" s="9"/>
       <c r="M58" s="4"/>
       <c r="N58" s="4"/>
       <c r="O58" s="4"/>
@@ -7237,18 +7560,32 @@
       <c r="AA58" s="4"/>
       <c r="AB58" s="4"/>
     </row>
-    <row r="59" spans="2:28" ht="12.75">
-      <c r="B59" s="4"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
-      <c r="G59" s="4"/>
-      <c r="H59" s="4"/>
-      <c r="I59" s="4"/>
-      <c r="J59" s="4"/>
-      <c r="K59" s="4"/>
-      <c r="L59" s="4"/>
+    <row r="59" spans="2:28" ht="27">
+      <c r="B59" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" s="9">
+        <v>2</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F59" s="9">
+        <v>2</v>
+      </c>
+      <c r="G59" s="9">
+        <v>0</v>
+      </c>
+      <c r="H59" s="9">
+        <v>2</v>
+      </c>
+      <c r="I59" s="9"/>
+      <c r="J59" s="9"/>
+      <c r="K59" s="9"/>
+      <c r="L59" s="9"/>
       <c r="M59" s="4"/>
       <c r="N59" s="4"/>
       <c r="O59" s="4"/>
@@ -7266,18 +7603,20 @@
       <c r="AA59" s="4"/>
       <c r="AB59" s="4"/>
     </row>
-    <row r="60" spans="2:28" ht="12.75">
-      <c r="B60" s="4"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
-      <c r="G60" s="4"/>
-      <c r="H60" s="4"/>
-      <c r="I60" s="4"/>
-      <c r="J60" s="4"/>
-      <c r="K60" s="4"/>
-      <c r="L60" s="4"/>
+    <row r="60" spans="2:28" ht="25.5">
+      <c r="B60" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C60" s="7"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="8"/>
+      <c r="K60" s="8"/>
+      <c r="L60" s="8"/>
       <c r="M60" s="4"/>
       <c r="N60" s="4"/>
       <c r="O60" s="4"/>
@@ -7295,18 +7634,32 @@
       <c r="AA60" s="4"/>
       <c r="AB60" s="4"/>
     </row>
-    <row r="61" spans="2:28" ht="12.75">
-      <c r="B61" s="4"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
-      <c r="I61" s="4"/>
-      <c r="J61" s="4"/>
-      <c r="K61" s="4"/>
-      <c r="L61" s="4"/>
+    <row r="61" spans="2:28" ht="40.5">
+      <c r="B61" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C61" s="9">
+        <v>1</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F61" s="9">
+        <v>1</v>
+      </c>
+      <c r="G61" s="9">
+        <v>0</v>
+      </c>
+      <c r="H61" s="9">
+        <v>2</v>
+      </c>
+      <c r="I61" s="9"/>
+      <c r="J61" s="9"/>
+      <c r="K61" s="9"/>
+      <c r="L61" s="9"/>
       <c r="M61" s="4"/>
       <c r="N61" s="4"/>
       <c r="O61" s="4"/>
@@ -7325,17 +7678,40 @@
       <c r="AB61" s="4"/>
     </row>
     <row r="62" spans="2:28" ht="12.75">
-      <c r="B62" s="4"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
-      <c r="J62" s="4"/>
-      <c r="K62" s="4"/>
-      <c r="L62" s="4"/>
+      <c r="B62" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5">
+        <f>SUM(F4:F59)</f>
+        <v>37.5</v>
+      </c>
+      <c r="G62" s="5">
+        <f>SUM(G4:G59)</f>
+        <v>23</v>
+      </c>
+      <c r="H62" s="5">
+        <f>SUM(H4:H59)</f>
+        <v>25.5</v>
+      </c>
+      <c r="I62" s="5">
+        <f>SUM(I4:I40)</f>
+        <v>0</v>
+      </c>
+      <c r="J62" s="5">
+        <f>SUM(J3:J40)</f>
+        <v>0</v>
+      </c>
+      <c r="K62" s="5">
+        <f>SUM(K9:K40)</f>
+        <v>0</v>
+      </c>
+      <c r="L62" s="5">
+        <f>SUM(L9:L40)</f>
+        <v>0</v>
+      </c>
       <c r="M62" s="4"/>
       <c r="N62" s="4"/>
       <c r="O62" s="4"/>
@@ -7353,7 +7729,7 @@
       <c r="AA62" s="4"/>
       <c r="AB62" s="4"/>
     </row>
-    <row r="63" spans="2:28" ht="12.75">
+    <row r="63" spans="2:28" ht="13.5">
       <c r="B63" s="4"/>
       <c r="C63" s="1"/>
       <c r="D63" s="4"/>
@@ -7382,7 +7758,7 @@
       <c r="AA63" s="4"/>
       <c r="AB63" s="4"/>
     </row>
-    <row r="64" spans="2:28" ht="12.75">
+    <row r="64" spans="2:28" ht="13.5">
       <c r="B64" s="4"/>
       <c r="C64" s="1"/>
       <c r="D64" s="4"/>
@@ -7411,7 +7787,7 @@
       <c r="AA64" s="4"/>
       <c r="AB64" s="4"/>
     </row>
-    <row r="65" spans="2:28" ht="12.75">
+    <row r="65" spans="2:28" ht="13.5">
       <c r="B65" s="4"/>
       <c r="C65" s="1"/>
       <c r="D65" s="4"/>
@@ -7440,8 +7816,10 @@
       <c r="AA65" s="4"/>
       <c r="AB65" s="4"/>
     </row>
-    <row r="66" spans="2:28" ht="12.75">
-      <c r="B66" s="4"/>
+    <row r="66" spans="2:28" ht="13.5">
+      <c r="B66" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="C66" s="1"/>
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
@@ -7469,8 +7847,10 @@
       <c r="AA66" s="4"/>
       <c r="AB66" s="4"/>
     </row>
-    <row r="67" spans="2:28" ht="12.75">
-      <c r="B67" s="4"/>
+    <row r="67" spans="2:28" ht="13.5">
+      <c r="B67" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="C67" s="1"/>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
@@ -7498,7 +7878,7 @@
       <c r="AA67" s="4"/>
       <c r="AB67" s="4"/>
     </row>
-    <row r="68" spans="2:28" ht="12.75">
+    <row r="68" spans="2:28" ht="13.5">
       <c r="B68" s="4"/>
       <c r="C68" s="1"/>
       <c r="D68" s="4"/>
@@ -7527,7 +7907,7 @@
       <c r="AA68" s="4"/>
       <c r="AB68" s="4"/>
     </row>
-    <row r="69" spans="2:28" ht="12.75">
+    <row r="69" spans="2:28" ht="13.5">
       <c r="B69" s="4"/>
       <c r="C69" s="1"/>
       <c r="D69" s="4"/>
@@ -7556,7 +7936,7 @@
       <c r="AA69" s="4"/>
       <c r="AB69" s="4"/>
     </row>
-    <row r="70" spans="2:28" ht="12.75">
+    <row r="70" spans="2:28" ht="13.5">
       <c r="B70" s="4"/>
       <c r="C70" s="1"/>
       <c r="D70" s="4"/>
@@ -7585,7 +7965,7 @@
       <c r="AA70" s="4"/>
       <c r="AB70" s="4"/>
     </row>
-    <row r="71" spans="2:28" ht="12.75">
+    <row r="71" spans="2:28" ht="13.5">
       <c r="B71" s="4"/>
       <c r="C71" s="1"/>
       <c r="D71" s="4"/>
@@ -7614,7 +7994,7 @@
       <c r="AA71" s="4"/>
       <c r="AB71" s="4"/>
     </row>
-    <row r="72" spans="2:28" ht="12.75">
+    <row r="72" spans="2:28" ht="13.5">
       <c r="B72" s="4"/>
       <c r="C72" s="1"/>
       <c r="D72" s="4"/>
@@ -7643,7 +8023,7 @@
       <c r="AA72" s="4"/>
       <c r="AB72" s="4"/>
     </row>
-    <row r="73" spans="2:28" ht="12.75">
+    <row r="73" spans="2:28" ht="13.5">
       <c r="B73" s="4"/>
       <c r="C73" s="1"/>
       <c r="D73" s="4"/>
@@ -7672,8 +8052,10 @@
       <c r="AA73" s="4"/>
       <c r="AB73" s="4"/>
     </row>
-    <row r="74" spans="2:28" ht="12.75">
-      <c r="B74" s="4"/>
+    <row r="74" spans="2:28" ht="13.5">
+      <c r="B74" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="C74" s="1"/>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
@@ -7701,8 +8083,10 @@
       <c r="AA74" s="4"/>
       <c r="AB74" s="4"/>
     </row>
-    <row r="75" spans="2:28" ht="12.75">
-      <c r="B75" s="4"/>
+    <row r="75" spans="2:28" ht="13.5">
+      <c r="B75" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="C75" s="1"/>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
@@ -7730,8 +8114,10 @@
       <c r="AA75" s="4"/>
       <c r="AB75" s="4"/>
     </row>
-    <row r="76" spans="2:28" ht="12.75">
-      <c r="B76" s="4"/>
+    <row r="76" spans="2:28" ht="13.5">
+      <c r="B76" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="C76" s="1"/>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
@@ -7759,7 +8145,7 @@
       <c r="AA76" s="4"/>
       <c r="AB76" s="4"/>
     </row>
-    <row r="77" spans="2:28" ht="12.75">
+    <row r="77" spans="2:28" ht="13.5">
       <c r="B77" s="4"/>
       <c r="C77" s="1"/>
       <c r="D77" s="4"/>
@@ -7788,7 +8174,7 @@
       <c r="AA77" s="4"/>
       <c r="AB77" s="4"/>
     </row>
-    <row r="78" spans="2:28" ht="12.75">
+    <row r="78" spans="2:28" ht="13.5">
       <c r="B78" s="4"/>
       <c r="C78" s="1"/>
       <c r="D78" s="4"/>
@@ -7817,7 +8203,7 @@
       <c r="AA78" s="4"/>
       <c r="AB78" s="4"/>
     </row>
-    <row r="79" spans="2:28" ht="12.75">
+    <row r="79" spans="2:28" ht="13.5">
       <c r="B79" s="4"/>
       <c r="C79" s="1"/>
       <c r="D79" s="4"/>
@@ -7846,7 +8232,7 @@
       <c r="AA79" s="4"/>
       <c r="AB79" s="4"/>
     </row>
-    <row r="80" spans="2:28" ht="12.75">
+    <row r="80" spans="2:28" ht="13.5">
       <c r="B80" s="4"/>
       <c r="C80" s="1"/>
       <c r="D80" s="4"/>
@@ -7875,7 +8261,7 @@
       <c r="AA80" s="4"/>
       <c r="AB80" s="4"/>
     </row>
-    <row r="81" spans="2:28" ht="12.75">
+    <row r="81" spans="2:28" ht="13.5">
       <c r="B81" s="4"/>
       <c r="C81" s="1"/>
       <c r="D81" s="4"/>
@@ -7904,7 +8290,7 @@
       <c r="AA81" s="4"/>
       <c r="AB81" s="4"/>
     </row>
-    <row r="82" spans="2:28" ht="12.75">
+    <row r="82" spans="2:28" ht="13.5">
       <c r="B82" s="4"/>
       <c r="C82" s="1"/>
       <c r="D82" s="4"/>
@@ -7933,7 +8319,7 @@
       <c r="AA82" s="4"/>
       <c r="AB82" s="4"/>
     </row>
-    <row r="83" spans="2:28" ht="12.75">
+    <row r="83" spans="2:28" ht="13.5">
       <c r="B83" s="4"/>
       <c r="C83" s="1"/>
       <c r="D83" s="4"/>
@@ -7962,7 +8348,7 @@
       <c r="AA83" s="4"/>
       <c r="AB83" s="4"/>
     </row>
-    <row r="84" spans="2:28" ht="12.75">
+    <row r="84" spans="2:28" ht="13.5">
       <c r="B84" s="4"/>
       <c r="C84" s="1"/>
       <c r="D84" s="4"/>
@@ -7991,7 +8377,7 @@
       <c r="AA84" s="4"/>
       <c r="AB84" s="4"/>
     </row>
-    <row r="85" spans="2:28" ht="12.75">
+    <row r="85" spans="2:28" ht="13.5">
       <c r="B85" s="4"/>
       <c r="C85" s="1"/>
       <c r="D85" s="4"/>
@@ -8020,7 +8406,7 @@
       <c r="AA85" s="4"/>
       <c r="AB85" s="4"/>
     </row>
-    <row r="86" spans="2:28" ht="12.75">
+    <row r="86" spans="2:28" ht="13.5">
       <c r="B86" s="4"/>
       <c r="C86" s="1"/>
       <c r="D86" s="4"/>
@@ -8049,7 +8435,7 @@
       <c r="AA86" s="4"/>
       <c r="AB86" s="4"/>
     </row>
-    <row r="87" spans="2:28" ht="12.75">
+    <row r="87" spans="2:28" ht="13.5">
       <c r="B87" s="4"/>
       <c r="C87" s="1"/>
       <c r="D87" s="4"/>
@@ -8078,7 +8464,7 @@
       <c r="AA87" s="4"/>
       <c r="AB87" s="4"/>
     </row>
-    <row r="88" spans="2:28" ht="12.75">
+    <row r="88" spans="2:28" ht="13.5">
       <c r="B88" s="4"/>
       <c r="C88" s="1"/>
       <c r="D88" s="4"/>
@@ -8107,7 +8493,7 @@
       <c r="AA88" s="4"/>
       <c r="AB88" s="4"/>
     </row>
-    <row r="89" spans="2:28" ht="12.75">
+    <row r="89" spans="2:28" ht="13.5">
       <c r="B89" s="4"/>
       <c r="C89" s="1"/>
       <c r="D89" s="4"/>
@@ -8136,7 +8522,7 @@
       <c r="AA89" s="4"/>
       <c r="AB89" s="4"/>
     </row>
-    <row r="90" spans="2:28" ht="12.75">
+    <row r="90" spans="2:28" ht="13.5">
       <c r="B90" s="4"/>
       <c r="C90" s="1"/>
       <c r="D90" s="4"/>
@@ -8165,7 +8551,7 @@
       <c r="AA90" s="4"/>
       <c r="AB90" s="4"/>
     </row>
-    <row r="91" spans="2:28" ht="12.75">
+    <row r="91" spans="2:28" ht="13.5">
       <c r="B91" s="4"/>
       <c r="C91" s="1"/>
       <c r="D91" s="4"/>
@@ -8194,7 +8580,7 @@
       <c r="AA91" s="4"/>
       <c r="AB91" s="4"/>
     </row>
-    <row r="92" spans="2:28" ht="12.75">
+    <row r="92" spans="2:28" ht="13.5">
       <c r="B92" s="4"/>
       <c r="C92" s="1"/>
       <c r="D92" s="4"/>
@@ -8223,7 +8609,7 @@
       <c r="AA92" s="4"/>
       <c r="AB92" s="4"/>
     </row>
-    <row r="93" spans="2:28" ht="12.75">
+    <row r="93" spans="2:28" ht="13.5">
       <c r="B93" s="4"/>
       <c r="C93" s="1"/>
       <c r="D93" s="4"/>
@@ -8252,7 +8638,7 @@
       <c r="AA93" s="4"/>
       <c r="AB93" s="4"/>
     </row>
-    <row r="94" spans="2:28" ht="12.75">
+    <row r="94" spans="2:28" ht="13.5">
       <c r="B94" s="4"/>
       <c r="C94" s="1"/>
       <c r="D94" s="4"/>
@@ -8281,7 +8667,7 @@
       <c r="AA94" s="4"/>
       <c r="AB94" s="4"/>
     </row>
-    <row r="95" spans="2:28" ht="12.75">
+    <row r="95" spans="2:28" ht="13.5">
       <c r="B95" s="4"/>
       <c r="C95" s="1"/>
       <c r="D95" s="4"/>
@@ -8310,7 +8696,7 @@
       <c r="AA95" s="4"/>
       <c r="AB95" s="4"/>
     </row>
-    <row r="96" spans="2:28" ht="12.75">
+    <row r="96" spans="2:28" ht="13.5">
       <c r="B96" s="4"/>
       <c r="C96" s="1"/>
       <c r="D96" s="4"/>
@@ -8339,7 +8725,7 @@
       <c r="AA96" s="4"/>
       <c r="AB96" s="4"/>
     </row>
-    <row r="97" spans="2:28" ht="12.75">
+    <row r="97" spans="2:28" ht="13.5">
       <c r="B97" s="4"/>
       <c r="C97" s="1"/>
       <c r="D97" s="4"/>
@@ -8368,7 +8754,7 @@
       <c r="AA97" s="4"/>
       <c r="AB97" s="4"/>
     </row>
-    <row r="98" spans="2:28" ht="12.75">
+    <row r="98" spans="2:28" ht="13.5">
       <c r="B98" s="4"/>
       <c r="C98" s="1"/>
       <c r="D98" s="4"/>
@@ -8397,7 +8783,7 @@
       <c r="AA98" s="4"/>
       <c r="AB98" s="4"/>
     </row>
-    <row r="99" spans="2:28" ht="12.75">
+    <row r="99" spans="2:28" ht="13.5">
       <c r="B99" s="4"/>
       <c r="C99" s="1"/>
       <c r="D99" s="4"/>
@@ -8426,7 +8812,7 @@
       <c r="AA99" s="4"/>
       <c r="AB99" s="4"/>
     </row>
-    <row r="100" spans="2:28" ht="12.75">
+    <row r="100" spans="2:28" ht="13.5">
       <c r="B100" s="4"/>
       <c r="C100" s="1"/>
       <c r="D100" s="4"/>
@@ -8455,7 +8841,7 @@
       <c r="AA100" s="4"/>
       <c r="AB100" s="4"/>
     </row>
-    <row r="101" spans="2:28" ht="12.75">
+    <row r="101" spans="2:28" ht="13.5">
       <c r="B101" s="4"/>
       <c r="C101" s="1"/>
       <c r="D101" s="4"/>
@@ -8484,7 +8870,7 @@
       <c r="AA101" s="4"/>
       <c r="AB101" s="4"/>
     </row>
-    <row r="102" spans="2:28" ht="12.75">
+    <row r="102" spans="2:28" ht="13.5">
       <c r="B102" s="4"/>
       <c r="C102" s="1"/>
       <c r="D102" s="4"/>
@@ -8513,7 +8899,7 @@
       <c r="AA102" s="4"/>
       <c r="AB102" s="4"/>
     </row>
-    <row r="103" spans="2:28" ht="12.75">
+    <row r="103" spans="2:28" ht="13.5">
       <c r="B103" s="4"/>
       <c r="C103" s="1"/>
       <c r="D103" s="4"/>
@@ -8542,7 +8928,7 @@
       <c r="AA103" s="4"/>
       <c r="AB103" s="4"/>
     </row>
-    <row r="104" spans="2:28" ht="12.75">
+    <row r="104" spans="2:28" ht="13.5">
       <c r="B104" s="4"/>
       <c r="C104" s="1"/>
       <c r="D104" s="4"/>
@@ -8571,7 +8957,7 @@
       <c r="AA104" s="4"/>
       <c r="AB104" s="4"/>
     </row>
-    <row r="105" spans="2:28" ht="12.75">
+    <row r="105" spans="2:28" ht="13.5">
       <c r="B105" s="4"/>
       <c r="C105" s="1"/>
       <c r="D105" s="4"/>
@@ -8600,7 +8986,7 @@
       <c r="AA105" s="4"/>
       <c r="AB105" s="4"/>
     </row>
-    <row r="106" spans="2:28" ht="12.75">
+    <row r="106" spans="2:28" ht="13.5">
       <c r="B106" s="4"/>
       <c r="C106" s="1"/>
       <c r="D106" s="4"/>
@@ -8629,7 +9015,7 @@
       <c r="AA106" s="4"/>
       <c r="AB106" s="4"/>
     </row>
-    <row r="107" spans="2:28" ht="12.75">
+    <row r="107" spans="2:28" ht="13.5">
       <c r="B107" s="4"/>
       <c r="C107" s="1"/>
       <c r="D107" s="4"/>
@@ -8658,7 +9044,7 @@
       <c r="AA107" s="4"/>
       <c r="AB107" s="4"/>
     </row>
-    <row r="108" spans="2:28" ht="12.75">
+    <row r="108" spans="2:28" ht="13.5">
       <c r="B108" s="4"/>
       <c r="C108" s="1"/>
       <c r="D108" s="4"/>
@@ -8687,7 +9073,7 @@
       <c r="AA108" s="4"/>
       <c r="AB108" s="4"/>
     </row>
-    <row r="109" spans="2:28" ht="12.75">
+    <row r="109" spans="2:28" ht="13.5">
       <c r="B109" s="4"/>
       <c r="C109" s="1"/>
       <c r="D109" s="4"/>
@@ -8716,7 +9102,7 @@
       <c r="AA109" s="4"/>
       <c r="AB109" s="4"/>
     </row>
-    <row r="110" spans="2:28" ht="12.75">
+    <row r="110" spans="2:28" ht="13.5">
       <c r="B110" s="4"/>
       <c r="C110" s="1"/>
       <c r="D110" s="4"/>
@@ -8745,7 +9131,7 @@
       <c r="AA110" s="4"/>
       <c r="AB110" s="4"/>
     </row>
-    <row r="111" spans="2:28" ht="12.75">
+    <row r="111" spans="2:28" ht="13.5">
       <c r="B111" s="4"/>
       <c r="C111" s="1"/>
       <c r="D111" s="4"/>
@@ -8774,7 +9160,7 @@
       <c r="AA111" s="4"/>
       <c r="AB111" s="4"/>
     </row>
-    <row r="112" spans="2:28" ht="12.75">
+    <row r="112" spans="2:28" ht="13.5">
       <c r="B112" s="4"/>
       <c r="C112" s="1"/>
       <c r="D112" s="4"/>
@@ -8803,7 +9189,7 @@
       <c r="AA112" s="4"/>
       <c r="AB112" s="4"/>
     </row>
-    <row r="113" spans="2:28" ht="12.75">
+    <row r="113" spans="2:28" ht="13.5">
       <c r="B113" s="4"/>
       <c r="C113" s="1"/>
       <c r="D113" s="4"/>
@@ -8832,7 +9218,7 @@
       <c r="AA113" s="4"/>
       <c r="AB113" s="4"/>
     </row>
-    <row r="114" spans="2:28" ht="12.75">
+    <row r="114" spans="2:28" ht="13.5">
       <c r="B114" s="4"/>
       <c r="C114" s="1"/>
       <c r="D114" s="4"/>
@@ -8861,7 +9247,7 @@
       <c r="AA114" s="4"/>
       <c r="AB114" s="4"/>
     </row>
-    <row r="115" spans="2:28" ht="12.75">
+    <row r="115" spans="2:28" ht="13.5">
       <c r="B115" s="4"/>
       <c r="C115" s="1"/>
       <c r="D115" s="4"/>
@@ -8890,7 +9276,7 @@
       <c r="AA115" s="4"/>
       <c r="AB115" s="4"/>
     </row>
-    <row r="116" spans="2:28" ht="12.75">
+    <row r="116" spans="2:28" ht="13.5">
       <c r="B116" s="4"/>
       <c r="C116" s="1"/>
       <c r="D116" s="4"/>
@@ -8919,7 +9305,7 @@
       <c r="AA116" s="4"/>
       <c r="AB116" s="4"/>
     </row>
-    <row r="117" spans="2:28" ht="12.75">
+    <row r="117" spans="2:28" ht="13.5">
       <c r="B117" s="4"/>
       <c r="C117" s="1"/>
       <c r="D117" s="4"/>
@@ -8948,7 +9334,7 @@
       <c r="AA117" s="4"/>
       <c r="AB117" s="4"/>
     </row>
-    <row r="118" spans="2:28" ht="12.75">
+    <row r="118" spans="2:28" ht="13.5">
       <c r="B118" s="4"/>
       <c r="C118" s="1"/>
       <c r="D118" s="4"/>
@@ -8977,7 +9363,7 @@
       <c r="AA118" s="4"/>
       <c r="AB118" s="4"/>
     </row>
-    <row r="119" spans="2:28" ht="12.75">
+    <row r="119" spans="2:28" ht="13.5">
       <c r="B119" s="4"/>
       <c r="C119" s="1"/>
       <c r="D119" s="4"/>
@@ -9006,7 +9392,7 @@
       <c r="AA119" s="4"/>
       <c r="AB119" s="4"/>
     </row>
-    <row r="120" spans="2:28" ht="12.75">
+    <row r="120" spans="2:28" ht="13.5">
       <c r="B120" s="4"/>
       <c r="C120" s="1"/>
       <c r="D120" s="4"/>
@@ -9035,7 +9421,7 @@
       <c r="AA120" s="4"/>
       <c r="AB120" s="4"/>
     </row>
-    <row r="121" spans="2:28" ht="12.75">
+    <row r="121" spans="2:28" ht="13.5">
       <c r="B121" s="4"/>
       <c r="C121" s="1"/>
       <c r="D121" s="4"/>
@@ -9064,7 +9450,7 @@
       <c r="AA121" s="4"/>
       <c r="AB121" s="4"/>
     </row>
-    <row r="122" spans="2:28" ht="12.75">
+    <row r="122" spans="2:28" ht="13.5">
       <c r="B122" s="4"/>
       <c r="C122" s="1"/>
       <c r="D122" s="4"/>
@@ -9093,7 +9479,7 @@
       <c r="AA122" s="4"/>
       <c r="AB122" s="4"/>
     </row>
-    <row r="123" spans="2:28" ht="12.75">
+    <row r="123" spans="2:28" ht="13.5">
       <c r="B123" s="4"/>
       <c r="C123" s="1"/>
       <c r="D123" s="4"/>
@@ -9122,7 +9508,7 @@
       <c r="AA123" s="4"/>
       <c r="AB123" s="4"/>
     </row>
-    <row r="124" spans="2:28" ht="12.75">
+    <row r="124" spans="2:28" ht="13.5">
       <c r="B124" s="4"/>
       <c r="C124" s="1"/>
       <c r="D124" s="4"/>
@@ -9151,7 +9537,7 @@
       <c r="AA124" s="4"/>
       <c r="AB124" s="4"/>
     </row>
-    <row r="125" spans="2:28" ht="12.75">
+    <row r="125" spans="2:28" ht="13.5">
       <c r="B125" s="4"/>
       <c r="C125" s="1"/>
       <c r="D125" s="4"/>
@@ -9180,7 +9566,7 @@
       <c r="AA125" s="4"/>
       <c r="AB125" s="4"/>
     </row>
-    <row r="126" spans="2:28" ht="12.75">
+    <row r="126" spans="2:28" ht="13.5">
       <c r="B126" s="4"/>
       <c r="C126" s="1"/>
       <c r="D126" s="4"/>
@@ -9192,8 +9578,24 @@
       <c r="J126" s="4"/>
       <c r="K126" s="4"/>
       <c r="L126" s="4"/>
-    </row>
-    <row r="127" spans="2:28" ht="12.75">
+      <c r="M126" s="4"/>
+      <c r="N126" s="4"/>
+      <c r="O126" s="4"/>
+      <c r="P126" s="4"/>
+      <c r="Q126" s="4"/>
+      <c r="R126" s="4"/>
+      <c r="S126" s="4"/>
+      <c r="T126" s="4"/>
+      <c r="U126" s="4"/>
+      <c r="V126" s="4"/>
+      <c r="W126" s="4"/>
+      <c r="X126" s="4"/>
+      <c r="Y126" s="4"/>
+      <c r="Z126" s="4"/>
+      <c r="AA126" s="4"/>
+      <c r="AB126" s="4"/>
+    </row>
+    <row r="127" spans="2:28" ht="13.5">
       <c r="B127" s="4"/>
       <c r="C127" s="1"/>
       <c r="D127" s="4"/>
@@ -9206,7 +9608,7 @@
       <c r="K127" s="4"/>
       <c r="L127" s="4"/>
     </row>
-    <row r="128" spans="2:28" ht="12.75">
+    <row r="128" spans="2:28" ht="13.5">
       <c r="B128" s="4"/>
       <c r="C128" s="1"/>
       <c r="D128" s="4"/>
@@ -9219,7 +9621,7 @@
       <c r="K128" s="4"/>
       <c r="L128" s="4"/>
     </row>
-    <row r="129" spans="2:12" ht="12.75">
+    <row r="129" spans="2:12" ht="13.5">
       <c r="B129" s="4"/>
       <c r="C129" s="1"/>
       <c r="D129" s="4"/>
@@ -9232,7 +9634,7 @@
       <c r="K129" s="4"/>
       <c r="L129" s="4"/>
     </row>
-    <row r="130" spans="2:12" ht="12.75">
+    <row r="130" spans="2:12" ht="13.5">
       <c r="B130" s="4"/>
       <c r="C130" s="1"/>
       <c r="D130" s="4"/>
@@ -9245,9 +9647,284 @@
       <c r="K130" s="4"/>
       <c r="L130" s="4"/>
     </row>
-    <row r="131" spans="2:12" ht="12.75"/>
-    <row r="132" spans="2:12" ht="12.75"/>
-    <row r="133" spans="2:12" ht="12.75"/>
+    <row r="131" spans="2:12" ht="13.5">
+      <c r="B131" s="4"/>
+      <c r="C131" s="1"/>
+      <c r="D131" s="4"/>
+      <c r="E131" s="4"/>
+      <c r="F131" s="4"/>
+      <c r="G131" s="4"/>
+      <c r="H131" s="4"/>
+      <c r="I131" s="4"/>
+      <c r="J131" s="4"/>
+      <c r="K131" s="4"/>
+      <c r="L131" s="4"/>
+    </row>
+    <row r="132" spans="2:12" ht="13.5">
+      <c r="B132" s="4"/>
+      <c r="C132" s="1"/>
+      <c r="D132" s="4"/>
+      <c r="E132" s="4"/>
+      <c r="F132" s="4"/>
+      <c r="G132" s="4"/>
+      <c r="H132" s="4"/>
+      <c r="I132" s="4"/>
+      <c r="J132" s="4"/>
+      <c r="K132" s="4"/>
+      <c r="L132" s="4"/>
+    </row>
+    <row r="133" spans="2:12" ht="13.5">
+      <c r="B133" s="4"/>
+      <c r="C133" s="1"/>
+      <c r="D133" s="4"/>
+      <c r="E133" s="4"/>
+      <c r="F133" s="4"/>
+      <c r="G133" s="4"/>
+      <c r="H133" s="4"/>
+      <c r="I133" s="4"/>
+      <c r="J133" s="4"/>
+      <c r="K133" s="4"/>
+      <c r="L133" s="4"/>
+    </row>
+    <row r="134" spans="2:12" ht="13.5">
+      <c r="B134" s="4"/>
+      <c r="C134" s="1"/>
+      <c r="D134" s="4"/>
+      <c r="E134" s="4"/>
+      <c r="F134" s="4"/>
+      <c r="G134" s="4"/>
+      <c r="H134" s="4"/>
+      <c r="I134" s="4"/>
+      <c r="J134" s="4"/>
+      <c r="K134" s="4"/>
+      <c r="L134" s="4"/>
+    </row>
+    <row r="135" spans="2:12" ht="13.5">
+      <c r="B135" s="4"/>
+      <c r="C135" s="1"/>
+      <c r="D135" s="4"/>
+      <c r="E135" s="4"/>
+      <c r="F135" s="4"/>
+      <c r="G135" s="4"/>
+      <c r="H135" s="4"/>
+      <c r="I135" s="4"/>
+      <c r="J135" s="4"/>
+      <c r="K135" s="4"/>
+      <c r="L135" s="4"/>
+    </row>
+    <row r="136" spans="2:12" ht="13.5">
+      <c r="B136" s="4"/>
+      <c r="C136" s="1"/>
+      <c r="D136" s="4"/>
+      <c r="E136" s="4"/>
+      <c r="F136" s="4"/>
+      <c r="G136" s="4"/>
+      <c r="H136" s="4"/>
+      <c r="I136" s="4"/>
+      <c r="J136" s="4"/>
+      <c r="K136" s="4"/>
+      <c r="L136" s="4"/>
+    </row>
+    <row r="137" spans="2:12" ht="13.5">
+      <c r="B137" s="4"/>
+      <c r="C137" s="1"/>
+      <c r="D137" s="4"/>
+      <c r="E137" s="4"/>
+      <c r="F137" s="4"/>
+      <c r="G137" s="4"/>
+      <c r="H137" s="4"/>
+      <c r="I137" s="4"/>
+      <c r="J137" s="4"/>
+      <c r="K137" s="4"/>
+      <c r="L137" s="4"/>
+    </row>
+    <row r="138" spans="2:12" ht="13.5">
+      <c r="B138" s="4"/>
+      <c r="C138" s="1"/>
+      <c r="D138" s="4"/>
+      <c r="E138" s="4"/>
+      <c r="F138" s="4"/>
+      <c r="G138" s="4"/>
+      <c r="H138" s="4"/>
+      <c r="I138" s="4"/>
+      <c r="J138" s="4"/>
+      <c r="K138" s="4"/>
+      <c r="L138" s="4"/>
+    </row>
+    <row r="139" spans="2:12" ht="13.5">
+      <c r="B139" s="4"/>
+      <c r="C139" s="1"/>
+      <c r="D139" s="4"/>
+      <c r="E139" s="4"/>
+      <c r="F139" s="4"/>
+      <c r="G139" s="4"/>
+      <c r="H139" s="4"/>
+      <c r="I139" s="4"/>
+      <c r="J139" s="4"/>
+      <c r="K139" s="4"/>
+      <c r="L139" s="4"/>
+    </row>
+    <row r="140" spans="2:12" ht="13.5">
+      <c r="B140" s="4"/>
+      <c r="C140" s="1"/>
+      <c r="D140" s="4"/>
+      <c r="E140" s="4"/>
+      <c r="F140" s="4"/>
+      <c r="G140" s="4"/>
+      <c r="H140" s="4"/>
+      <c r="I140" s="4"/>
+      <c r="J140" s="4"/>
+      <c r="K140" s="4"/>
+      <c r="L140" s="4"/>
+    </row>
+    <row r="141" spans="2:12" ht="13.5">
+      <c r="B141" s="4"/>
+      <c r="C141" s="1"/>
+      <c r="D141" s="4"/>
+      <c r="E141" s="4"/>
+      <c r="F141" s="4"/>
+      <c r="G141" s="4"/>
+      <c r="H141" s="4"/>
+      <c r="I141" s="4"/>
+      <c r="J141" s="4"/>
+      <c r="K141" s="4"/>
+      <c r="L141" s="4"/>
+    </row>
+    <row r="142" spans="2:12" ht="13.5">
+      <c r="B142" s="4"/>
+      <c r="C142" s="1"/>
+      <c r="D142" s="4"/>
+      <c r="E142" s="4"/>
+      <c r="F142" s="4"/>
+      <c r="G142" s="4"/>
+      <c r="H142" s="4"/>
+      <c r="I142" s="4"/>
+      <c r="J142" s="4"/>
+      <c r="K142" s="4"/>
+      <c r="L142" s="4"/>
+    </row>
+    <row r="143" spans="2:12" ht="13.5">
+      <c r="B143" s="4"/>
+      <c r="C143" s="1"/>
+      <c r="D143" s="4"/>
+      <c r="E143" s="4"/>
+      <c r="F143" s="4"/>
+      <c r="G143" s="4"/>
+      <c r="H143" s="4"/>
+      <c r="I143" s="4"/>
+      <c r="J143" s="4"/>
+      <c r="K143" s="4"/>
+      <c r="L143" s="4"/>
+    </row>
+    <row r="144" spans="2:12" ht="13.5">
+      <c r="B144" s="4"/>
+      <c r="C144" s="1"/>
+      <c r="D144" s="4"/>
+      <c r="E144" s="4"/>
+      <c r="F144" s="4"/>
+      <c r="G144" s="4"/>
+      <c r="H144" s="4"/>
+      <c r="I144" s="4"/>
+      <c r="J144" s="4"/>
+      <c r="K144" s="4"/>
+      <c r="L144" s="4"/>
+    </row>
+    <row r="145" spans="2:12" ht="13.5">
+      <c r="B145" s="4"/>
+      <c r="C145" s="1"/>
+      <c r="D145" s="4"/>
+      <c r="E145" s="4"/>
+      <c r="F145" s="4"/>
+      <c r="G145" s="4"/>
+      <c r="H145" s="4"/>
+      <c r="I145" s="4"/>
+      <c r="J145" s="4"/>
+      <c r="K145" s="4"/>
+      <c r="L145" s="4"/>
+    </row>
+    <row r="146" spans="2:12" ht="13.5">
+      <c r="B146" s="4"/>
+      <c r="C146" s="1"/>
+      <c r="D146" s="4"/>
+      <c r="E146" s="4"/>
+      <c r="F146" s="4"/>
+      <c r="G146" s="4"/>
+      <c r="H146" s="4"/>
+      <c r="I146" s="4"/>
+      <c r="J146" s="4"/>
+      <c r="K146" s="4"/>
+      <c r="L146" s="4"/>
+    </row>
+    <row r="147" spans="2:12" ht="13.5">
+      <c r="B147" s="4"/>
+      <c r="C147" s="1"/>
+      <c r="D147" s="4"/>
+      <c r="E147" s="4"/>
+      <c r="F147" s="4"/>
+      <c r="G147" s="4"/>
+      <c r="H147" s="4"/>
+      <c r="I147" s="4"/>
+      <c r="J147" s="4"/>
+      <c r="K147" s="4"/>
+      <c r="L147" s="4"/>
+    </row>
+    <row r="148" spans="2:12" ht="13.5">
+      <c r="B148" s="4"/>
+      <c r="C148" s="1"/>
+      <c r="D148" s="4"/>
+      <c r="E148" s="4"/>
+      <c r="F148" s="4"/>
+      <c r="G148" s="4"/>
+      <c r="H148" s="4"/>
+      <c r="I148" s="4"/>
+      <c r="J148" s="4"/>
+      <c r="K148" s="4"/>
+      <c r="L148" s="4"/>
+    </row>
+    <row r="149" spans="2:12" ht="13.5">
+      <c r="B149" s="4"/>
+      <c r="C149" s="1"/>
+      <c r="D149" s="4"/>
+      <c r="E149" s="4"/>
+      <c r="F149" s="4"/>
+      <c r="G149" s="4"/>
+      <c r="H149" s="4"/>
+      <c r="I149" s="4"/>
+      <c r="J149" s="4"/>
+      <c r="K149" s="4"/>
+      <c r="L149" s="4"/>
+    </row>
+    <row r="150" spans="2:12" ht="13.5">
+      <c r="B150" s="4"/>
+      <c r="C150" s="1"/>
+      <c r="D150" s="4"/>
+      <c r="E150" s="4"/>
+      <c r="F150" s="4"/>
+      <c r="G150" s="4"/>
+      <c r="H150" s="4"/>
+      <c r="I150" s="4"/>
+      <c r="J150" s="4"/>
+      <c r="K150" s="4"/>
+      <c r="L150" s="4"/>
+    </row>
+    <row r="151" spans="2:12" ht="13.5">
+      <c r="B151" s="4"/>
+      <c r="C151" s="1"/>
+      <c r="D151" s="4"/>
+      <c r="E151" s="4"/>
+      <c r="F151" s="4"/>
+      <c r="G151" s="4"/>
+      <c r="H151" s="4"/>
+      <c r="I151" s="4"/>
+      <c r="J151" s="4"/>
+      <c r="K151" s="4"/>
+      <c r="L151" s="4"/>
+    </row>
+    <row r="152" spans="2:12" ht="13.5"/>
+    <row r="153" spans="2:12" ht="13.5"/>
+    <row r="154" spans="2:12" ht="13.5"/>
+    <row r="155" spans="2:12" ht="13.5"/>
+    <row r="156" spans="2:12" ht="13.5"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:V1"/>
@@ -9278,7 +9955,7 @@
   <sheetData>
     <row r="2" spans="2:2" ht="90">
       <c r="B2" s="10" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated sprint backlog for wednesday
New sprint backlog with information up to date as of wednesday
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint2_Backlog-1.xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint2_Backlog-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_186\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F359C66F-8C0F-4DDF-A3B4-5EC0580D5EF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E95A775-1AE4-4F6D-B713-2DD2960146CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="-Disclaimer-" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Agile Sprint 2 Backlog '!$B$2:$V$29</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Agile Sprint 2 Backlog '!$B$2:$V$30</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Sprint Backlog'!$B$2:$V$28</definedName>
   </definedNames>
   <calcPr calcId="191028" calcCompleted="0"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="85">
   <si>
     <t>AGILE SPRINT BACKLOG TEMPLATE WITH BURNDOWN CHART</t>
   </si>
@@ -155,6 +155,12 @@
     <t>R.C/H.Z</t>
   </si>
   <si>
+    <t>Cost is shown in 2dp</t>
+  </si>
+  <si>
+    <t>C.H</t>
+  </si>
+  <si>
     <t>Generation Of testing</t>
   </si>
   <si>
@@ -188,13 +194,13 @@
     <t>CSS animations to help useability</t>
   </si>
   <si>
-    <t>C.H</t>
-  </si>
-  <si>
     <t>Implementing animations in website</t>
   </si>
   <si>
     <t>Table cell click behaves like marker click</t>
+  </si>
+  <si>
+    <t>View cost in table</t>
   </si>
   <si>
     <t>Create test functions for search SQL procedures via distance.</t>
@@ -222,6 +228,9 @@
   </si>
   <si>
     <t>Recieving cost of procedure from SQL</t>
+  </si>
+  <si>
+    <t>Changing colour of map marker</t>
   </si>
   <si>
     <t>As a client, I want to see the facilities rating when I click it's marker</t>
@@ -260,6 +269,12 @@
     <t>Returning a hospital list with distances associated with each hospital relative to users's location.</t>
   </si>
   <si>
+    <t>Sort hosptial distance by shortest to longest hospital distance away from user</t>
+  </si>
+  <si>
+    <t>Returning a hospital list with shortest distances first.</t>
+  </si>
+  <si>
     <t>Day 1 Notes:</t>
   </si>
   <si>
@@ -269,7 +284,7 @@
     <t>Day 2 Notes:</t>
   </si>
   <si>
-    <t>C.H - New user stories were considered so I updated the sprint backlog accordingly</t>
+    <t>C.H - New user stories were considered so I updated the product backlog accordingly</t>
   </si>
   <si>
     <t>R.C - Updated Methods to reflect more accurate information, Meaning re-evaluation of esitmated time</t>
@@ -450,7 +465,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -488,6 +503,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -789,15 +805,30 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Agile Sprint 2 Backlog '!$F$62:$G$62</c:f>
+              <c:f>'Agile Sprint 2 Backlog '!$F$65:$L$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>37.5</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1006,7 +1037,7 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>812800</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>431800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1366,7 +1397,7 @@
   <dimension ref="B1:AB124"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="B7" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -5383,11 +5414,11 @@
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AB156"/>
+  <dimension ref="B1:AB164"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.15"/>
@@ -6070,18 +6101,22 @@
         <v>39</v>
       </c>
       <c r="C18" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="9"/>
+        <v>24</v>
+      </c>
+      <c r="F18" s="9">
+        <v>1</v>
+      </c>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
+      <c r="I18" s="9">
+        <v>0.5</v>
+      </c>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
@@ -6102,22 +6137,26 @@
       <c r="AA18" s="4"/>
       <c r="AB18" s="4"/>
     </row>
-    <row r="19" spans="2:28" ht="38.25">
-      <c r="B19" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8">
-        <v>1</v>
-      </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
+    <row r="19" spans="2:28" ht="25.15" customHeight="1">
+      <c r="B19" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="9">
+        <v>2</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
@@ -6135,30 +6174,22 @@
       <c r="AA19" s="4"/>
       <c r="AB19" s="4"/>
     </row>
-    <row r="20" spans="2:28" ht="25.15" customHeight="1">
-      <c r="B20" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="9">
+    <row r="20" spans="2:28" ht="38.25">
+      <c r="B20" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8">
         <v>1</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="9">
-        <v>2</v>
-      </c>
-      <c r="G20" s="9">
-        <v>5</v>
-      </c>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
@@ -6180,11 +6211,21 @@
       <c r="B21" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
+      <c r="C21" s="9">
+        <v>1</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="9">
+        <v>2</v>
+      </c>
+      <c r="G21" s="9">
+        <v>5</v>
+      </c>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
@@ -6209,7 +6250,7 @@
     </row>
     <row r="22" spans="2:28" ht="25.15" customHeight="1">
       <c r="B22" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -6240,7 +6281,7 @@
     </row>
     <row r="23" spans="2:28" ht="25.15" customHeight="1">
       <c r="B23" s="9" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -6270,19 +6311,19 @@
       <c r="AB23" s="4"/>
     </row>
     <row r="24" spans="2:28" ht="25.15" customHeight="1">
-      <c r="B24" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
+      <c r="B24" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
@@ -6301,31 +6342,19 @@
       <c r="AB24" s="4"/>
     </row>
     <row r="25" spans="2:28" ht="25.15" customHeight="1">
-      <c r="B25" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="9">
-        <v>1</v>
-      </c>
-      <c r="D25" s="9" t="s">
+      <c r="B25" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E25" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F25" s="9">
-        <v>1</v>
-      </c>
-      <c r="G25" s="9">
-        <v>1</v>
-      </c>
-      <c r="H25" s="9">
-        <v>0</v>
-      </c>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
@@ -6345,14 +6374,26 @@
     </row>
     <row r="26" spans="2:28" ht="25.15" customHeight="1">
       <c r="B26" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
+        <v>48</v>
+      </c>
+      <c r="C26" s="9">
+        <v>1</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="9">
+        <v>1</v>
+      </c>
+      <c r="G26" s="9">
+        <v>1</v>
+      </c>
+      <c r="H26" s="9">
+        <v>0</v>
+      </c>
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
@@ -6376,7 +6417,7 @@
     </row>
     <row r="27" spans="2:28" ht="25.15" customHeight="1">
       <c r="B27" s="9" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -6436,20 +6477,20 @@
       <c r="AA28" s="4"/>
       <c r="AB28" s="4"/>
     </row>
-    <row r="29" spans="2:28" ht="34.9" customHeight="1">
-      <c r="B29" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
+    <row r="29" spans="2:28" ht="25.15" customHeight="1">
+      <c r="B29" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
@@ -6467,32 +6508,20 @@
       <c r="AA29" s="4"/>
       <c r="AB29" s="4"/>
     </row>
-    <row r="30" spans="2:28" ht="18" customHeight="1">
-      <c r="B30" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" s="9">
-        <v>1</v>
-      </c>
-      <c r="D30" s="9" t="s">
+    <row r="30" spans="2:28" ht="34.9" customHeight="1">
+      <c r="B30" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E30" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F30" s="9">
-        <v>1</v>
-      </c>
-      <c r="G30" s="9">
-        <v>2</v>
-      </c>
-      <c r="H30" s="9">
-        <v>1</v>
-      </c>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
@@ -6510,27 +6539,27 @@
       <c r="AA30" s="4"/>
       <c r="AB30" s="4"/>
     </row>
-    <row r="31" spans="2:28" ht="14.25" customHeight="1">
+    <row r="31" spans="2:28" ht="18" customHeight="1">
       <c r="B31" s="9" t="s">
         <v>51</v>
       </c>
       <c r="C31" s="9">
+        <v>1</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="9">
+        <v>1</v>
+      </c>
+      <c r="G31" s="9">
         <v>2</v>
       </c>
-      <c r="D31" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F31" s="9">
-        <v>2</v>
-      </c>
-      <c r="G31" s="9">
-        <v>5</v>
-      </c>
       <c r="H31" s="9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
@@ -6553,7 +6582,7 @@
       <c r="AA31" s="4"/>
       <c r="AB31" s="4"/>
     </row>
-    <row r="32" spans="2:28" ht="13.5">
+    <row r="32" spans="2:28" ht="14.25" customHeight="1">
       <c r="B32" s="9" t="s">
         <v>52</v>
       </c>
@@ -6561,21 +6590,23 @@
         <v>2</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F32" s="9">
         <v>2</v>
       </c>
       <c r="G32" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H32" s="9">
-        <v>3</v>
-      </c>
-      <c r="I32" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="I32" s="9">
+        <v>2</v>
+      </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
       <c r="L32" s="9"/>
@@ -6596,17 +6627,31 @@
       <c r="AA32" s="4"/>
       <c r="AB32" s="4"/>
     </row>
-    <row r="33" spans="2:28" ht="12.75">
+    <row r="33" spans="2:28" ht="13.5">
       <c r="B33" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
+        <v>53</v>
+      </c>
+      <c r="C33" s="9">
+        <v>2</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" s="9">
+        <v>2</v>
+      </c>
+      <c r="G33" s="9">
+        <v>0</v>
+      </c>
+      <c r="H33" s="9">
+        <v>3</v>
+      </c>
+      <c r="I33" s="9">
+        <v>2</v>
+      </c>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
       <c r="L33" s="9"/>
@@ -6627,15 +6672,27 @@
       <c r="AA33" s="4"/>
       <c r="AB33" s="4"/>
     </row>
-    <row r="34" spans="2:28" ht="12.75">
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
+    <row r="34" spans="2:28" ht="13.5">
+      <c r="B34" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="9">
+        <v>1</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" s="9">
+        <v>1</v>
+      </c>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
+      <c r="I34" s="9">
+        <v>0.5</v>
+      </c>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
       <c r="L34" s="9"/>
@@ -6656,20 +6713,18 @@
       <c r="AA34" s="4"/>
       <c r="AB34" s="4"/>
     </row>
-    <row r="35" spans="2:28" ht="34.9" customHeight="1">
-      <c r="B35" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
+    <row r="35" spans="2:28" ht="13.5">
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
@@ -6687,32 +6742,20 @@
       <c r="AA35" s="4"/>
       <c r="AB35" s="4"/>
     </row>
-    <row r="36" spans="2:28" ht="12.75">
-      <c r="B36" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C36" s="9">
-        <v>1</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F36" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="G36" s="9">
-        <v>0</v>
-      </c>
-      <c r="H36" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="I36" s="9"/>
-      <c r="J36" s="9"/>
-      <c r="K36" s="9"/>
-      <c r="L36" s="9"/>
+    <row r="36" spans="2:28" ht="34.9" customHeight="1">
+      <c r="B36" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="7"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
@@ -6730,15 +6773,15 @@
       <c r="AA36" s="4"/>
       <c r="AB36" s="4"/>
     </row>
-    <row r="37" spans="2:28" ht="14.25" customHeight="1">
+    <row r="37" spans="2:28" ht="27">
       <c r="B37" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C37" s="9">
         <v>1</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E37" s="9" t="s">
         <v>24</v>
@@ -6773,15 +6816,15 @@
       <c r="AA37" s="4"/>
       <c r="AB37" s="4"/>
     </row>
-    <row r="38" spans="2:28" ht="25.5">
+    <row r="38" spans="2:28" ht="14.25" customHeight="1">
       <c r="B38" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C38" s="9">
         <v>1</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E38" s="9" t="s">
         <v>24</v>
@@ -6816,23 +6859,27 @@
       <c r="AA38" s="4"/>
       <c r="AB38" s="4"/>
     </row>
-    <row r="39" spans="2:28" ht="13.5">
-      <c r="B39" s="9"/>
+    <row r="39" spans="2:28" ht="27">
+      <c r="B39" s="9" t="s">
+        <v>58</v>
+      </c>
       <c r="C39" s="9">
         <v>1</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="F39" s="9">
         <v>0.5</v>
       </c>
-      <c r="G39" s="9"/>
+      <c r="G39" s="9">
+        <v>0</v>
+      </c>
       <c r="H39" s="9">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I39" s="9"/>
       <c r="J39" s="9"/>
@@ -6864,14 +6911,14 @@
         <v>30</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="F40" s="9">
         <v>0.5</v>
       </c>
       <c r="G40" s="9"/>
       <c r="H40" s="9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I40" s="9"/>
       <c r="J40" s="9"/>
@@ -6894,20 +6941,28 @@
       <c r="AA40" s="4"/>
       <c r="AB40" s="4"/>
     </row>
-    <row r="41" spans="2:28" ht="26.25" customHeight="1">
-      <c r="B41" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
+    <row r="41" spans="2:28" ht="13.5">
+      <c r="B41" s="9"/>
+      <c r="C41" s="9">
+        <v>1</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F41" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
@@ -6925,30 +6980,20 @@
       <c r="AA41" s="4"/>
       <c r="AB41" s="4"/>
     </row>
-    <row r="42" spans="2:28" ht="25.5">
-      <c r="B42" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C42" s="9">
-        <v>1</v>
-      </c>
-      <c r="D42" s="9" t="s">
+    <row r="42" spans="2:28" ht="26.25" customHeight="1">
+      <c r="B42" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E42" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F42" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="G42" s="9">
-        <v>1</v>
-      </c>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-      <c r="J42" s="9"/>
-      <c r="K42" s="9"/>
-      <c r="L42" s="9"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
@@ -6966,7 +7011,7 @@
       <c r="AA42" s="4"/>
       <c r="AB42" s="4"/>
     </row>
-    <row r="43" spans="2:28" ht="12.75">
+    <row r="43" spans="2:28" ht="27">
       <c r="B43" s="9" t="s">
         <v>61</v>
       </c>
@@ -6974,16 +7019,16 @@
         <v>1</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F43" s="9">
         <v>0.5</v>
       </c>
       <c r="G43" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43" s="9"/>
       <c r="I43" s="9"/>
@@ -7007,16 +7052,28 @@
       <c r="AA43" s="4"/>
       <c r="AB43" s="4"/>
     </row>
-    <row r="44" spans="2:28" ht="12.75">
+    <row r="44" spans="2:28" ht="13.5">
       <c r="B44" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
+        <v>63</v>
+      </c>
+      <c r="C44" s="9">
+        <v>1</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F44" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G44" s="9">
+        <v>0</v>
+      </c>
+      <c r="H44" s="9">
+        <v>1</v>
+      </c>
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
@@ -7038,16 +7095,28 @@
       <c r="AA44" s="4"/>
       <c r="AB44" s="4"/>
     </row>
-    <row r="45" spans="2:28" ht="12.75">
+    <row r="45" spans="2:28" ht="13.5">
       <c r="B45" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
+        <v>64</v>
+      </c>
+      <c r="C45" s="9">
+        <v>1</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F45" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="G45" s="9">
+        <v>0</v>
+      </c>
+      <c r="H45" s="9">
+        <v>1.5</v>
+      </c>
       <c r="I45" s="9"/>
       <c r="J45" s="9"/>
       <c r="K45" s="9"/>
@@ -7069,20 +7138,20 @@
       <c r="AA45" s="4"/>
       <c r="AB45" s="4"/>
     </row>
-    <row r="46" spans="2:28" ht="25.5">
-      <c r="B46" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C46" s="7"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="8"/>
-      <c r="K46" s="8"/>
-      <c r="L46" s="8"/>
+    <row r="46" spans="2:28" ht="13.5">
+      <c r="B46" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
       <c r="M46" s="4"/>
       <c r="N46" s="4"/>
       <c r="O46" s="4"/>
@@ -7101,29 +7170,19 @@
       <c r="AB46" s="4"/>
     </row>
     <row r="47" spans="2:28" ht="25.5">
-      <c r="B47" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C47" s="9">
-        <v>1</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F47" s="9">
-        <v>1</v>
-      </c>
-      <c r="G47" s="9">
-        <v>1</v>
-      </c>
-      <c r="H47" s="9"/>
-      <c r="I47" s="9"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="9"/>
-      <c r="L47" s="9"/>
+      <c r="B47" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="7"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="8"/>
       <c r="M47" s="4"/>
       <c r="N47" s="4"/>
       <c r="O47" s="4"/>
@@ -7141,24 +7200,24 @@
       <c r="AA47" s="4"/>
       <c r="AB47" s="4"/>
     </row>
-    <row r="48" spans="2:28" ht="12.75">
+    <row r="48" spans="2:28" ht="27">
       <c r="B48" s="9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C48" s="9">
         <v>1</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F48" s="9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G48" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48" s="9"/>
       <c r="I48" s="9"/>
@@ -7182,16 +7241,28 @@
       <c r="AA48" s="4"/>
       <c r="AB48" s="4"/>
     </row>
-    <row r="49" spans="2:28" ht="12.75">
+    <row r="49" spans="2:28" ht="13.5">
       <c r="B49" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
+        <v>67</v>
+      </c>
+      <c r="C49" s="9">
+        <v>1</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F49" s="9">
+        <v>1</v>
+      </c>
+      <c r="G49" s="9">
+        <v>0</v>
+      </c>
+      <c r="H49" s="9">
+        <v>2</v>
+      </c>
       <c r="I49" s="9"/>
       <c r="J49" s="9"/>
       <c r="K49" s="9"/>
@@ -7213,7 +7284,7 @@
       <c r="AA49" s="4"/>
       <c r="AB49" s="4"/>
     </row>
-    <row r="50" spans="2:28" ht="12.75">
+    <row r="50" spans="2:28" ht="13.5">
       <c r="B50" s="9" t="s">
         <v>14</v>
       </c>
@@ -7244,20 +7315,20 @@
       <c r="AA50" s="4"/>
       <c r="AB50" s="4"/>
     </row>
-    <row r="51" spans="2:28" ht="25.5">
-      <c r="B51" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C51" s="7"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="8"/>
-      <c r="J51" s="8"/>
-      <c r="K51" s="8"/>
-      <c r="L51" s="8"/>
+    <row r="51" spans="2:28" ht="13.5">
+      <c r="B51" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="9"/>
+      <c r="L51" s="9"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
       <c r="O51" s="4"/>
@@ -7275,32 +7346,20 @@
       <c r="AA51" s="4"/>
       <c r="AB51" s="4"/>
     </row>
-    <row r="52" spans="2:28" ht="12.75">
-      <c r="B52" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C52" s="9">
-        <v>1</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F52" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="G52" s="9">
-        <v>0</v>
-      </c>
-      <c r="H52" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="I52" s="9"/>
-      <c r="J52" s="9"/>
-      <c r="K52" s="9"/>
-      <c r="L52" s="9"/>
+    <row r="52" spans="2:28" ht="25.5">
+      <c r="B52" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52" s="7"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8"/>
+      <c r="L52" s="8"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
       <c r="O52" s="4"/>
@@ -7318,15 +7377,15 @@
       <c r="AA52" s="4"/>
       <c r="AB52" s="4"/>
     </row>
-    <row r="53" spans="2:28" ht="25.5">
+    <row r="53" spans="2:28" ht="27">
       <c r="B53" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C53" s="9">
         <v>1</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E53" s="9" t="s">
         <v>33</v>
@@ -7361,15 +7420,15 @@
       <c r="AA53" s="4"/>
       <c r="AB53" s="4"/>
     </row>
-    <row r="54" spans="2:28" ht="25.5">
+    <row r="54" spans="2:28" ht="27">
       <c r="B54" s="9" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C54" s="9">
         <v>1</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E54" s="9" t="s">
         <v>33</v>
@@ -7406,23 +7465,25 @@
     </row>
     <row r="55" spans="2:28" ht="27">
       <c r="B55" s="9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C55" s="9">
         <v>1</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="F55" s="9">
         <v>0.5</v>
       </c>
-      <c r="G55" s="9"/>
+      <c r="G55" s="9">
+        <v>0</v>
+      </c>
       <c r="H55" s="9">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I55" s="9"/>
       <c r="J55" s="9"/>
@@ -7447,7 +7508,7 @@
     </row>
     <row r="56" spans="2:28" ht="27">
       <c r="B56" s="9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C56" s="9">
         <v>1</v>
@@ -7456,14 +7517,14 @@
         <v>30</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="F56" s="9">
         <v>0.5</v>
       </c>
       <c r="G56" s="9"/>
       <c r="H56" s="9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I56" s="9"/>
       <c r="J56" s="9"/>
@@ -7486,20 +7547,30 @@
       <c r="AA56" s="4"/>
       <c r="AB56" s="4"/>
     </row>
-    <row r="57" spans="2:28" ht="25.5">
-      <c r="B57" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C57" s="7"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="8"/>
-      <c r="G57" s="8"/>
-      <c r="H57" s="8"/>
-      <c r="I57" s="8"/>
-      <c r="J57" s="8"/>
-      <c r="K57" s="8"/>
-      <c r="L57" s="8"/>
+    <row r="57" spans="2:28" ht="27">
+      <c r="B57" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C57" s="9">
+        <v>1</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F57" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9"/>
+      <c r="K57" s="9"/>
+      <c r="L57" s="9"/>
       <c r="M57" s="4"/>
       <c r="N57" s="4"/>
       <c r="O57" s="4"/>
@@ -7517,32 +7588,20 @@
       <c r="AA57" s="4"/>
       <c r="AB57" s="4"/>
     </row>
-    <row r="58" spans="2:28" ht="13.5">
-      <c r="B58" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C58" s="9">
-        <v>1</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F58" s="9">
-        <v>1</v>
-      </c>
-      <c r="G58" s="9">
-        <v>0</v>
-      </c>
-      <c r="H58" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="I58" s="9"/>
-      <c r="J58" s="9"/>
-      <c r="K58" s="9"/>
-      <c r="L58" s="9"/>
+    <row r="58" spans="2:28" ht="25.5">
+      <c r="B58" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C58" s="7"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="8"/>
+      <c r="L58" s="8"/>
       <c r="M58" s="4"/>
       <c r="N58" s="4"/>
       <c r="O58" s="4"/>
@@ -7560,27 +7619,27 @@
       <c r="AA58" s="4"/>
       <c r="AB58" s="4"/>
     </row>
-    <row r="59" spans="2:28" ht="27">
+    <row r="59" spans="2:28" ht="13.5">
       <c r="B59" s="9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C59" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E59" s="9" t="s">
         <v>24</v>
       </c>
       <c r="F59" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G59" s="9">
         <v>0</v>
       </c>
       <c r="H59" s="9">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="I59" s="9"/>
       <c r="J59" s="9"/>
@@ -7603,20 +7662,32 @@
       <c r="AA59" s="4"/>
       <c r="AB59" s="4"/>
     </row>
-    <row r="60" spans="2:28" ht="25.5">
-      <c r="B60" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C60" s="7"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
-      <c r="F60" s="8"/>
-      <c r="G60" s="8"/>
-      <c r="H60" s="8"/>
-      <c r="I60" s="8"/>
-      <c r="J60" s="8"/>
-      <c r="K60" s="8"/>
-      <c r="L60" s="8"/>
+    <row r="60" spans="2:28" ht="27">
+      <c r="B60" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="9">
+        <v>2</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F60" s="9">
+        <v>2</v>
+      </c>
+      <c r="G60" s="9">
+        <v>0</v>
+      </c>
+      <c r="H60" s="9">
+        <v>2</v>
+      </c>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9"/>
+      <c r="K60" s="9"/>
+      <c r="L60" s="9"/>
       <c r="M60" s="4"/>
       <c r="N60" s="4"/>
       <c r="O60" s="4"/>
@@ -7634,32 +7705,20 @@
       <c r="AA60" s="4"/>
       <c r="AB60" s="4"/>
     </row>
-    <row r="61" spans="2:28" ht="40.5">
-      <c r="B61" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C61" s="9">
-        <v>1</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F61" s="9">
-        <v>1</v>
-      </c>
-      <c r="G61" s="9">
-        <v>0</v>
-      </c>
-      <c r="H61" s="9">
-        <v>2</v>
-      </c>
-      <c r="I61" s="9"/>
-      <c r="J61" s="9"/>
-      <c r="K61" s="9"/>
-      <c r="L61" s="9"/>
+    <row r="61" spans="2:28" ht="25.5">
+      <c r="B61" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C61" s="7"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="8"/>
+      <c r="J61" s="8"/>
+      <c r="K61" s="8"/>
+      <c r="L61" s="8"/>
       <c r="M61" s="4"/>
       <c r="N61" s="4"/>
       <c r="O61" s="4"/>
@@ -7677,41 +7736,34 @@
       <c r="AA61" s="4"/>
       <c r="AB61" s="4"/>
     </row>
-    <row r="62" spans="2:28" ht="12.75">
-      <c r="B62" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="5">
-        <f>SUM(F4:F59)</f>
-        <v>37.5</v>
-      </c>
-      <c r="G62" s="5">
-        <f>SUM(G4:G59)</f>
-        <v>23</v>
-      </c>
-      <c r="H62" s="5">
-        <f>SUM(H4:H59)</f>
-        <v>25.5</v>
-      </c>
-      <c r="I62" s="5">
-        <f>SUM(I4:I40)</f>
+    <row r="62" spans="2:28" ht="40.5">
+      <c r="B62" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C62" s="9">
+        <v>1</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F62" s="9">
+        <v>1</v>
+      </c>
+      <c r="G62" s="9">
         <v>0</v>
       </c>
-      <c r="J62" s="5">
-        <f>SUM(J3:J40)</f>
-        <v>0</v>
-      </c>
-      <c r="K62" s="5">
-        <f>SUM(K9:K40)</f>
-        <v>0</v>
-      </c>
-      <c r="L62" s="5">
-        <f>SUM(L9:L40)</f>
-        <v>0</v>
-      </c>
+      <c r="H62" s="9">
+        <v>2</v>
+      </c>
+      <c r="I62" s="9">
+        <v>2</v>
+      </c>
+      <c r="J62" s="9"/>
+      <c r="K62" s="9"/>
+      <c r="L62" s="9"/>
       <c r="M62" s="4"/>
       <c r="N62" s="4"/>
       <c r="O62" s="4"/>
@@ -7729,18 +7781,20 @@
       <c r="AA62" s="4"/>
       <c r="AB62" s="4"/>
     </row>
-    <row r="63" spans="2:28" ht="13.5">
-      <c r="B63" s="4"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
-      <c r="K63" s="4"/>
-      <c r="L63" s="4"/>
+    <row r="63" spans="2:28" ht="38.25">
+      <c r="B63" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C63" s="7"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="8"/>
+      <c r="K63" s="8"/>
+      <c r="L63" s="8"/>
       <c r="M63" s="4"/>
       <c r="N63" s="4"/>
       <c r="O63" s="4"/>
@@ -7758,18 +7812,34 @@
       <c r="AA63" s="4"/>
       <c r="AB63" s="4"/>
     </row>
-    <row r="64" spans="2:28" ht="13.5">
-      <c r="B64" s="4"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="4"/>
-      <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
-      <c r="K64" s="4"/>
-      <c r="L64" s="4"/>
+    <row r="64" spans="2:28" ht="27">
+      <c r="B64" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C64" s="9">
+        <v>2</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F64" s="9">
+        <v>1</v>
+      </c>
+      <c r="G64" s="9">
+        <v>0</v>
+      </c>
+      <c r="H64" s="9">
+        <v>2</v>
+      </c>
+      <c r="I64" s="9">
+        <v>2</v>
+      </c>
+      <c r="J64" s="9"/>
+      <c r="K64" s="9"/>
+      <c r="L64" s="9"/>
       <c r="M64" s="4"/>
       <c r="N64" s="4"/>
       <c r="O64" s="4"/>
@@ -7787,18 +7857,41 @@
       <c r="AA64" s="4"/>
       <c r="AB64" s="4"/>
     </row>
-    <row r="65" spans="2:28" ht="13.5">
-      <c r="B65" s="4"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
-      <c r="H65" s="4"/>
-      <c r="I65" s="4"/>
-      <c r="J65" s="4"/>
-      <c r="K65" s="4"/>
-      <c r="L65" s="4"/>
+    <row r="65" spans="2:28" ht="12.75">
+      <c r="B65" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5">
+        <f>SUM(F4:F64)</f>
+        <v>43.5</v>
+      </c>
+      <c r="G65" s="5">
+        <f>SUM(G4:G64)</f>
+        <v>23</v>
+      </c>
+      <c r="H65" s="5">
+        <f>SUM(H4:H64)</f>
+        <v>34</v>
+      </c>
+      <c r="I65" s="5">
+        <f>SUM(I4:I64)</f>
+        <v>9</v>
+      </c>
+      <c r="J65" s="5">
+        <f>SUM(J3:J64)</f>
+        <v>0</v>
+      </c>
+      <c r="K65" s="5">
+        <f>SUM(K9:K64)</f>
+        <v>0</v>
+      </c>
+      <c r="L65" s="5">
+        <f>SUM(L9:L64)</f>
+        <v>0</v>
+      </c>
       <c r="M65" s="4"/>
       <c r="N65" s="4"/>
       <c r="O65" s="4"/>
@@ -7817,19 +7910,17 @@
       <c r="AB65" s="4"/>
     </row>
     <row r="66" spans="2:28" ht="13.5">
-      <c r="B66" s="4" t="s">
-        <v>74</v>
-      </c>
+      <c r="B66" s="17"/>
       <c r="C66" s="1"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4"/>
-      <c r="G66" s="4"/>
-      <c r="H66" s="4"/>
-      <c r="I66" s="4"/>
-      <c r="J66" s="4"/>
-      <c r="K66" s="4"/>
-      <c r="L66" s="4"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
+      <c r="F66" s="17"/>
+      <c r="G66" s="17"/>
+      <c r="H66" s="17"/>
+      <c r="I66" s="17"/>
+      <c r="J66" s="17"/>
+      <c r="K66" s="17"/>
+      <c r="L66" s="17"/>
       <c r="M66" s="4"/>
       <c r="N66" s="4"/>
       <c r="O66" s="4"/>
@@ -7848,19 +7939,17 @@
       <c r="AB66" s="4"/>
     </row>
     <row r="67" spans="2:28" ht="13.5">
-      <c r="B67" s="4" t="s">
-        <v>75</v>
-      </c>
+      <c r="B67" s="17"/>
       <c r="C67" s="1"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="4"/>
-      <c r="G67" s="4"/>
-      <c r="H67" s="4"/>
-      <c r="I67" s="4"/>
-      <c r="J67" s="4"/>
-      <c r="K67" s="4"/>
-      <c r="L67" s="4"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="17"/>
+      <c r="F67" s="17"/>
+      <c r="G67" s="17"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="17"/>
+      <c r="J67" s="17"/>
+      <c r="K67" s="17"/>
+      <c r="L67" s="17"/>
       <c r="M67" s="4"/>
       <c r="N67" s="4"/>
       <c r="O67" s="4"/>
@@ -7879,17 +7968,17 @@
       <c r="AB67" s="4"/>
     </row>
     <row r="68" spans="2:28" ht="13.5">
-      <c r="B68" s="4"/>
+      <c r="B68" s="17"/>
       <c r="C68" s="1"/>
-      <c r="D68" s="4"/>
-      <c r="E68" s="4"/>
-      <c r="F68" s="4"/>
-      <c r="G68" s="4"/>
-      <c r="H68" s="4"/>
-      <c r="I68" s="4"/>
-      <c r="J68" s="4"/>
-      <c r="K68" s="4"/>
-      <c r="L68" s="4"/>
+      <c r="D68" s="17"/>
+      <c r="E68" s="17"/>
+      <c r="F68" s="17"/>
+      <c r="G68" s="17"/>
+      <c r="H68" s="17"/>
+      <c r="I68" s="17"/>
+      <c r="J68" s="17"/>
+      <c r="K68" s="17"/>
+      <c r="L68" s="17"/>
       <c r="M68" s="4"/>
       <c r="N68" s="4"/>
       <c r="O68" s="4"/>
@@ -7908,17 +7997,19 @@
       <c r="AB68" s="4"/>
     </row>
     <row r="69" spans="2:28" ht="13.5">
-      <c r="B69" s="4"/>
+      <c r="B69" s="17" t="s">
+        <v>79</v>
+      </c>
       <c r="C69" s="1"/>
-      <c r="D69" s="4"/>
-      <c r="E69" s="4"/>
-      <c r="F69" s="4"/>
-      <c r="G69" s="4"/>
-      <c r="H69" s="4"/>
-      <c r="I69" s="4"/>
-      <c r="J69" s="4"/>
-      <c r="K69" s="4"/>
-      <c r="L69" s="4"/>
+      <c r="D69" s="17"/>
+      <c r="E69" s="17"/>
+      <c r="F69" s="17"/>
+      <c r="G69" s="17"/>
+      <c r="H69" s="17"/>
+      <c r="I69" s="17"/>
+      <c r="J69" s="17"/>
+      <c r="K69" s="17"/>
+      <c r="L69" s="17"/>
       <c r="M69" s="4"/>
       <c r="N69" s="4"/>
       <c r="O69" s="4"/>
@@ -7937,7 +8028,9 @@
       <c r="AB69" s="4"/>
     </row>
     <row r="70" spans="2:28" ht="13.5">
-      <c r="B70" s="4"/>
+      <c r="B70" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="C70" s="1"/>
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
@@ -8053,9 +8146,7 @@
       <c r="AB73" s="4"/>
     </row>
     <row r="74" spans="2:28" ht="13.5">
-      <c r="B74" s="4" t="s">
-        <v>76</v>
-      </c>
+      <c r="B74" s="4"/>
       <c r="C74" s="1"/>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
@@ -8084,9 +8175,7 @@
       <c r="AB74" s="4"/>
     </row>
     <row r="75" spans="2:28" ht="13.5">
-      <c r="B75" s="4" t="s">
-        <v>77</v>
-      </c>
+      <c r="B75" s="4"/>
       <c r="C75" s="1"/>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
@@ -8115,9 +8204,7 @@
       <c r="AB75" s="4"/>
     </row>
     <row r="76" spans="2:28" ht="13.5">
-      <c r="B76" s="4" t="s">
-        <v>78</v>
-      </c>
+      <c r="B76" s="4"/>
       <c r="C76" s="1"/>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
@@ -8146,7 +8233,9 @@
       <c r="AB76" s="4"/>
     </row>
     <row r="77" spans="2:28" ht="13.5">
-      <c r="B77" s="4"/>
+      <c r="B77" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="C77" s="1"/>
       <c r="D77" s="4"/>
       <c r="E77" s="4"/>
@@ -8175,7 +8264,9 @@
       <c r="AB77" s="4"/>
     </row>
     <row r="78" spans="2:28" ht="13.5">
-      <c r="B78" s="4"/>
+      <c r="B78" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="C78" s="1"/>
       <c r="D78" s="4"/>
       <c r="E78" s="4"/>
@@ -8204,7 +8295,9 @@
       <c r="AB78" s="4"/>
     </row>
     <row r="79" spans="2:28" ht="13.5">
-      <c r="B79" s="4"/>
+      <c r="B79" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="C79" s="1"/>
       <c r="D79" s="4"/>
       <c r="E79" s="4"/>
@@ -9491,22 +9584,6 @@
       <c r="J123" s="4"/>
       <c r="K123" s="4"/>
       <c r="L123" s="4"/>
-      <c r="M123" s="4"/>
-      <c r="N123" s="4"/>
-      <c r="O123" s="4"/>
-      <c r="P123" s="4"/>
-      <c r="Q123" s="4"/>
-      <c r="R123" s="4"/>
-      <c r="S123" s="4"/>
-      <c r="T123" s="4"/>
-      <c r="U123" s="4"/>
-      <c r="V123" s="4"/>
-      <c r="W123" s="4"/>
-      <c r="X123" s="4"/>
-      <c r="Y123" s="4"/>
-      <c r="Z123" s="4"/>
-      <c r="AA123" s="4"/>
-      <c r="AB123" s="4"/>
     </row>
     <row r="124" spans="2:28" ht="13.5">
       <c r="B124" s="4"/>
@@ -9520,22 +9597,6 @@
       <c r="J124" s="4"/>
       <c r="K124" s="4"/>
       <c r="L124" s="4"/>
-      <c r="M124" s="4"/>
-      <c r="N124" s="4"/>
-      <c r="O124" s="4"/>
-      <c r="P124" s="4"/>
-      <c r="Q124" s="4"/>
-      <c r="R124" s="4"/>
-      <c r="S124" s="4"/>
-      <c r="T124" s="4"/>
-      <c r="U124" s="4"/>
-      <c r="V124" s="4"/>
-      <c r="W124" s="4"/>
-      <c r="X124" s="4"/>
-      <c r="Y124" s="4"/>
-      <c r="Z124" s="4"/>
-      <c r="AA124" s="4"/>
-      <c r="AB124" s="4"/>
     </row>
     <row r="125" spans="2:28" ht="13.5">
       <c r="B125" s="4"/>
@@ -9549,22 +9610,6 @@
       <c r="J125" s="4"/>
       <c r="K125" s="4"/>
       <c r="L125" s="4"/>
-      <c r="M125" s="4"/>
-      <c r="N125" s="4"/>
-      <c r="O125" s="4"/>
-      <c r="P125" s="4"/>
-      <c r="Q125" s="4"/>
-      <c r="R125" s="4"/>
-      <c r="S125" s="4"/>
-      <c r="T125" s="4"/>
-      <c r="U125" s="4"/>
-      <c r="V125" s="4"/>
-      <c r="W125" s="4"/>
-      <c r="X125" s="4"/>
-      <c r="Y125" s="4"/>
-      <c r="Z125" s="4"/>
-      <c r="AA125" s="4"/>
-      <c r="AB125" s="4"/>
     </row>
     <row r="126" spans="2:28" ht="13.5">
       <c r="B126" s="4"/>
@@ -9578,22 +9623,6 @@
       <c r="J126" s="4"/>
       <c r="K126" s="4"/>
       <c r="L126" s="4"/>
-      <c r="M126" s="4"/>
-      <c r="N126" s="4"/>
-      <c r="O126" s="4"/>
-      <c r="P126" s="4"/>
-      <c r="Q126" s="4"/>
-      <c r="R126" s="4"/>
-      <c r="S126" s="4"/>
-      <c r="T126" s="4"/>
-      <c r="U126" s="4"/>
-      <c r="V126" s="4"/>
-      <c r="W126" s="4"/>
-      <c r="X126" s="4"/>
-      <c r="Y126" s="4"/>
-      <c r="Z126" s="4"/>
-      <c r="AA126" s="4"/>
-      <c r="AB126" s="4"/>
     </row>
     <row r="127" spans="2:28" ht="13.5">
       <c r="B127" s="4"/>
@@ -9920,11 +9949,55 @@
       <c r="K151" s="4"/>
       <c r="L151" s="4"/>
     </row>
-    <row r="152" spans="2:12" ht="13.5"/>
-    <row r="153" spans="2:12" ht="13.5"/>
-    <row r="154" spans="2:12" ht="13.5"/>
+    <row r="152" spans="2:12" ht="13.5">
+      <c r="B152" s="4"/>
+      <c r="C152" s="1"/>
+      <c r="D152" s="4"/>
+      <c r="E152" s="4"/>
+      <c r="F152" s="4"/>
+      <c r="G152" s="4"/>
+      <c r="H152" s="4"/>
+      <c r="I152" s="4"/>
+      <c r="J152" s="4"/>
+      <c r="K152" s="4"/>
+      <c r="L152" s="4"/>
+    </row>
+    <row r="153" spans="2:12" ht="13.5">
+      <c r="B153" s="4"/>
+      <c r="C153" s="1"/>
+      <c r="D153" s="4"/>
+      <c r="E153" s="4"/>
+      <c r="F153" s="4"/>
+      <c r="G153" s="4"/>
+      <c r="H153" s="4"/>
+      <c r="I153" s="4"/>
+      <c r="J153" s="4"/>
+      <c r="K153" s="4"/>
+      <c r="L153" s="4"/>
+    </row>
+    <row r="154" spans="2:12" ht="13.5">
+      <c r="B154" s="4"/>
+      <c r="C154" s="1"/>
+      <c r="D154" s="4"/>
+      <c r="E154" s="4"/>
+      <c r="F154" s="4"/>
+      <c r="G154" s="4"/>
+      <c r="H154" s="4"/>
+      <c r="I154" s="4"/>
+      <c r="J154" s="4"/>
+      <c r="K154" s="4"/>
+      <c r="L154" s="4"/>
+    </row>
     <row r="155" spans="2:12" ht="13.5"/>
     <row r="156" spans="2:12" ht="13.5"/>
+    <row r="157" spans="2:12" ht="13.5"/>
+    <row r="158" spans="2:12" ht="13.5"/>
+    <row r="159" spans="2:12" ht="13.5"/>
+    <row r="160" spans="2:12" ht="13.5"/>
+    <row r="161" ht="13.5"/>
+    <row r="162" ht="13.5"/>
+    <row r="163" ht="13.5"/>
+    <row r="164" ht="13.5"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:V1"/>
@@ -9955,7 +10028,7 @@
   <sheetData>
     <row r="2" spans="2:2" ht="90">
       <c r="B2" s="10" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -9965,6 +10038,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000A45299412FDFE49916D3B2BC7498215" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="528d0d9d29f55c94d322eb3857adfb37">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7b8fda29-18fb-4238-bb7d-7bcb176bce57" xmlns:ns4="c00e3565-1744-4d61-af64-fc54f2252c20" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8027d906c71b20e95020a61b0ffa4a2b" ns3:_="" ns4:_="">
     <xsd:import namespace="7b8fda29-18fb-4238-bb7d-7bcb176bce57"/>
@@ -10155,23 +10243,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E12810E-FE41-41C7-A55A-C2E990FA16A4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30A64F61-EAC8-4AA1-B802-5855346DCB32}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10179,5 +10252,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30A64F61-EAC8-4AA1-B802-5855346DCB32}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E12810E-FE41-41C7-A55A-C2E990FA16A4}"/>
 </file>
</xml_diff>